<commit_message>
Refactored newLoanCreation function to handle optional data
</commit_message>
<xml_diff>
--- a/test_Data/Loan.xlsx
+++ b/test_Data/Loan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NagaSaiSriharshaKara\Desktop\PRMG\test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF146F3A-DDE2-4EE6-8245-8F55514CAA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D414A6C1-C391-488A-8E6A-DB9389E023B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="2" xr2:uid="{162BA2F1-E430-497A-A5CB-FF5EFBDA5730}"/>
   </bookViews>
@@ -16,8 +16,9 @@
     <sheet name="Borrower Information" sheetId="1" r:id="rId1"/>
     <sheet name="Property Title" sheetId="3" r:id="rId2"/>
     <sheet name="Loans Info" sheetId="6" r:id="rId3"/>
-    <sheet name="Employment Income" sheetId="5" r:id="rId4"/>
-    <sheet name="Loan Information" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
+    <sheet name="Employment Income" sheetId="5" r:id="rId5"/>
+    <sheet name="Loan Information" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="283">
   <si>
     <t>First Name</t>
   </si>
@@ -815,6 +816,78 @@
   </si>
   <si>
     <t>Co Military Service 1</t>
+  </si>
+  <si>
+    <t>Interview Option 3</t>
+  </si>
+  <si>
+    <t>Ethnicity 3</t>
+  </si>
+  <si>
+    <t>Race 3</t>
+  </si>
+  <si>
+    <t>Sex 3</t>
+  </si>
+  <si>
+    <t>First Name 3</t>
+  </si>
+  <si>
+    <t>Middle Name 3</t>
+  </si>
+  <si>
+    <t>Last Name 3</t>
+  </si>
+  <si>
+    <t>Vesting Type 3</t>
+  </si>
+  <si>
+    <t>SSN 3</t>
+  </si>
+  <si>
+    <t>Petr</t>
+  </si>
+  <si>
+    <t>Yan</t>
+  </si>
+  <si>
+    <t>Street Address 3</t>
+  </si>
+  <si>
+    <t>Zip 3</t>
+  </si>
+  <si>
+    <t>Years 3</t>
+  </si>
+  <si>
+    <t>Months 3</t>
+  </si>
+  <si>
+    <t>Citizenship 3</t>
+  </si>
+  <si>
+    <t>Dob 3</t>
+  </si>
+  <si>
+    <t>Marital Status 3</t>
+  </si>
+  <si>
+    <t>Home Phone 3</t>
+  </si>
+  <si>
+    <t>Work Phone 3</t>
+  </si>
+  <si>
+    <t>Cell Phone 3</t>
+  </si>
+  <si>
+    <t>Email 3</t>
+  </si>
+  <si>
+    <t>petr@gmail.com</t>
+  </si>
+  <si>
+    <t>245 street</t>
   </si>
 </sst>
 </file>
@@ -960,7 +1033,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -990,20 +1063,20 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1828,10 +1901,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{442BC2CD-504F-478A-8238-60A656DB3140}">
-  <dimension ref="A1:JW15"/>
+  <dimension ref="A1:JR12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1974,9 +2047,28 @@
     <col min="137" max="137" width="28.1796875" bestFit="1" customWidth="1"/>
     <col min="138" max="138" width="28.90625" bestFit="1" customWidth="1"/>
     <col min="139" max="139" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="145" max="145" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="155" max="155" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="157" max="157" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="11" bestFit="1" customWidth="1"/>
+    <col min="159" max="159" width="16.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:283" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:278" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>192</v>
       </c>
@@ -2394,157 +2486,192 @@
       <c r="EI1" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="EJ1" s="15"/>
-      <c r="EK1" s="15"/>
-      <c r="EL1" s="15"/>
-      <c r="EM1" s="15"/>
-      <c r="EN1" s="15"/>
-      <c r="EO1" s="15"/>
-      <c r="EP1" s="15"/>
-      <c r="EQ1" s="15"/>
-      <c r="ER1" s="15"/>
-      <c r="ES1" s="15"/>
-      <c r="ET1" s="15"/>
-      <c r="EU1" s="15"/>
-      <c r="EV1" s="15"/>
-      <c r="EW1" s="15"/>
-      <c r="EX1" s="15"/>
-      <c r="EY1" s="15"/>
-      <c r="EZ1" s="15"/>
-      <c r="FA1" s="15"/>
-      <c r="FB1" s="15"/>
-      <c r="FC1" s="15"/>
-      <c r="FD1" s="15"/>
-      <c r="FE1" s="15"/>
-      <c r="FF1" s="15"/>
-      <c r="FG1" s="15"/>
-      <c r="FH1" s="15"/>
-      <c r="FI1" s="15"/>
-      <c r="FJ1" s="15"/>
-      <c r="FK1" s="15"/>
-      <c r="FL1" s="15"/>
-      <c r="FM1" s="15"/>
-      <c r="FN1" s="15"/>
-      <c r="FO1" s="15"/>
-      <c r="FP1" s="15"/>
-      <c r="FQ1" s="15"/>
-      <c r="FR1" s="15"/>
-      <c r="FS1" s="15"/>
-      <c r="FT1" s="15"/>
-      <c r="FU1" s="15"/>
-      <c r="FV1" s="15"/>
-      <c r="FW1" s="15"/>
-      <c r="FX1" s="15"/>
-      <c r="FY1" s="15"/>
-      <c r="FZ1" s="15"/>
-      <c r="GA1" s="15"/>
-      <c r="GB1" s="15"/>
-      <c r="GC1" s="15"/>
-      <c r="GD1" s="15"/>
-      <c r="GE1" s="15"/>
-      <c r="GF1" s="15"/>
-      <c r="GG1" s="15"/>
-      <c r="GH1" s="15"/>
-      <c r="GI1" s="15"/>
-      <c r="GJ1" s="15"/>
-      <c r="GK1" s="15"/>
-      <c r="GL1" s="15"/>
-      <c r="GM1" s="15"/>
-      <c r="GN1" s="15"/>
-      <c r="GO1" s="15"/>
-      <c r="GP1" s="15"/>
-      <c r="GQ1" s="15"/>
-      <c r="GR1" s="15"/>
-      <c r="GS1" s="15"/>
-      <c r="GT1" s="15"/>
-      <c r="GU1" s="15"/>
-      <c r="GV1" s="15"/>
-      <c r="GW1" s="15"/>
-      <c r="GX1" s="15"/>
-      <c r="GY1" s="15"/>
-      <c r="GZ1" s="15"/>
-      <c r="HA1" s="15"/>
-      <c r="HB1" s="15"/>
-      <c r="HC1" s="15"/>
-      <c r="HD1" s="15"/>
-      <c r="HE1" s="15"/>
-      <c r="HF1" s="15"/>
-      <c r="HG1" s="15"/>
-      <c r="HH1" s="15"/>
-      <c r="HI1" s="15"/>
-      <c r="HJ1" s="15"/>
-      <c r="HK1" s="15"/>
-      <c r="HL1" s="15"/>
-      <c r="HM1" s="15"/>
-      <c r="HN1" s="15"/>
-      <c r="HO1" s="15"/>
-      <c r="HP1" s="15"/>
-      <c r="HQ1" s="15"/>
-      <c r="HR1" s="15"/>
-      <c r="HS1" s="15"/>
-      <c r="HT1" s="15"/>
-      <c r="HU1" s="15"/>
-      <c r="HV1" s="15"/>
-      <c r="HW1" s="15"/>
-      <c r="HX1" s="15"/>
-      <c r="HY1" s="15"/>
-      <c r="HZ1" s="15"/>
-      <c r="IA1" s="15"/>
-      <c r="IB1" s="15"/>
-      <c r="IC1" s="15"/>
-      <c r="ID1" s="15"/>
-      <c r="IE1" s="15"/>
-      <c r="IF1" s="15"/>
-      <c r="IG1" s="15"/>
-      <c r="IH1" s="15"/>
-      <c r="II1" s="15"/>
-      <c r="IJ1" s="15"/>
-      <c r="IK1" s="15"/>
-      <c r="IL1" s="15"/>
-      <c r="IM1" s="15"/>
-      <c r="IN1" s="15"/>
-      <c r="IO1" s="15"/>
-      <c r="IP1" s="15"/>
-      <c r="IQ1" s="15"/>
-      <c r="IR1" s="15"/>
-      <c r="IS1" s="15"/>
-      <c r="IT1" s="15"/>
-      <c r="IU1" s="15"/>
-      <c r="IV1" s="15"/>
-      <c r="IW1" s="15"/>
-      <c r="IX1" s="15"/>
-      <c r="IY1" s="15"/>
-      <c r="IZ1" s="15"/>
-      <c r="JA1" s="15"/>
-      <c r="JB1" s="15"/>
-      <c r="JC1" s="15"/>
-      <c r="JD1" s="15"/>
-      <c r="JE1" s="15"/>
-      <c r="JF1" s="15"/>
-      <c r="JG1" s="15"/>
-      <c r="JH1" s="15"/>
-      <c r="JI1" s="15"/>
-      <c r="JJ1" s="15"/>
-      <c r="JK1" s="15"/>
-      <c r="JL1" s="15"/>
-      <c r="JM1" s="15"/>
-      <c r="JN1" s="15"/>
-      <c r="JO1" s="15"/>
-      <c r="JP1" s="15"/>
-      <c r="JQ1" s="15"/>
-      <c r="JR1" s="15"/>
-      <c r="JS1" s="15"/>
-      <c r="JT1" s="15"/>
-      <c r="JU1" s="15"/>
-      <c r="JV1" s="15"/>
-      <c r="JW1" s="15"/>
+      <c r="EJ1" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="EK1" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="EL1" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="EM1" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="EN1" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="EO1" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="EP1" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="EQ1" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="ER1" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="ES1" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="ET1" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="EU1" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="EV1" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="EW1" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="EX1" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="EY1" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="EZ1" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="FA1" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="FB1" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="FC1" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="FD1"/>
+      <c r="FE1"/>
+      <c r="FF1"/>
+      <c r="FG1"/>
+      <c r="FH1"/>
+      <c r="FI1"/>
+      <c r="FJ1"/>
+      <c r="FK1"/>
+      <c r="FL1"/>
+      <c r="FM1"/>
+      <c r="FN1"/>
+      <c r="FO1"/>
+      <c r="FP1"/>
+      <c r="FQ1"/>
+      <c r="FR1"/>
+      <c r="FS1"/>
+      <c r="FT1"/>
+      <c r="FU1"/>
+      <c r="FV1"/>
+      <c r="FW1"/>
+      <c r="FX1"/>
+      <c r="FY1"/>
+      <c r="FZ1"/>
+      <c r="GA1"/>
+      <c r="GB1"/>
+      <c r="GC1"/>
+      <c r="GD1"/>
+      <c r="GE1"/>
+      <c r="GF1"/>
+      <c r="GG1"/>
+      <c r="GH1"/>
+      <c r="GI1"/>
+      <c r="GJ1"/>
+      <c r="GK1"/>
+      <c r="GL1"/>
+      <c r="GM1"/>
+      <c r="GN1"/>
+      <c r="GO1"/>
+      <c r="GP1"/>
+      <c r="GQ1"/>
+      <c r="GR1"/>
+      <c r="GS1"/>
+      <c r="GT1"/>
+      <c r="GU1"/>
+      <c r="GV1"/>
+      <c r="GW1"/>
+      <c r="GX1"/>
+      <c r="GY1"/>
+      <c r="GZ1"/>
+      <c r="HA1"/>
+      <c r="HB1"/>
+      <c r="HC1"/>
+      <c r="HD1"/>
+      <c r="HE1"/>
+      <c r="HF1"/>
+      <c r="HG1"/>
+      <c r="HH1"/>
+      <c r="HI1"/>
+      <c r="HJ1"/>
+      <c r="HK1"/>
+      <c r="HL1"/>
+      <c r="HM1"/>
+      <c r="HN1"/>
+      <c r="HO1"/>
+      <c r="HP1"/>
+      <c r="HQ1"/>
+      <c r="HR1"/>
+      <c r="HS1"/>
+      <c r="HT1"/>
+      <c r="HU1"/>
+      <c r="HV1"/>
+      <c r="HW1"/>
+      <c r="HX1"/>
+      <c r="HY1"/>
+      <c r="HZ1"/>
+      <c r="IA1"/>
+      <c r="IB1"/>
+      <c r="IC1"/>
+      <c r="ID1"/>
+      <c r="IE1"/>
+      <c r="IF1"/>
+      <c r="IG1"/>
+      <c r="IH1"/>
+      <c r="II1"/>
+      <c r="IJ1"/>
+      <c r="IK1"/>
+      <c r="IL1"/>
+      <c r="IM1"/>
+      <c r="IN1"/>
+      <c r="IO1"/>
+      <c r="IP1"/>
+      <c r="IQ1"/>
+      <c r="IR1"/>
+      <c r="IS1"/>
+      <c r="IT1"/>
+      <c r="IU1"/>
+      <c r="IV1"/>
+      <c r="IW1"/>
+      <c r="IX1"/>
+      <c r="IY1"/>
+      <c r="IZ1"/>
+      <c r="JA1"/>
+      <c r="JB1"/>
+      <c r="JC1"/>
+      <c r="JD1"/>
+      <c r="JE1"/>
+      <c r="JF1"/>
+      <c r="JG1"/>
+      <c r="JH1"/>
+      <c r="JI1"/>
+      <c r="JJ1"/>
+      <c r="JK1"/>
+      <c r="JL1"/>
+      <c r="JM1"/>
+      <c r="JN1"/>
+      <c r="JO1"/>
+      <c r="JP1"/>
+      <c r="JQ1"/>
+      <c r="JR1"/>
     </row>
-    <row r="2" spans="1:283" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:278" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>203</v>
@@ -2591,7 +2718,7 @@
       <c r="Q2" s="1">
         <v>2893930406</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="20" t="s">
         <v>206</v>
       </c>
       <c r="S2" s="5">
@@ -2666,25 +2793,25 @@
       <c r="AP2" s="13">
         <v>4091997</v>
       </c>
-      <c r="AQ2" s="15" t="s">
+      <c r="AQ2" t="s">
         <v>220</v>
       </c>
-      <c r="AR2" s="15" t="s">
+      <c r="AR2" t="s">
         <v>240</v>
       </c>
-      <c r="AS2" s="15" t="s">
+      <c r="AS2" t="s">
         <v>227</v>
       </c>
-      <c r="AT2" s="17" t="s">
+      <c r="AT2" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="AU2" s="16" t="s">
+      <c r="AU2" t="s">
         <v>246</v>
       </c>
-      <c r="AV2" s="17" t="s">
+      <c r="AV2" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="AW2" s="21" t="s">
+      <c r="AW2" s="15" t="s">
         <v>246</v>
       </c>
       <c r="AX2" t="s">
@@ -2702,8 +2829,8 @@
       <c r="BB2" s="1">
         <v>189309305</v>
       </c>
-      <c r="BC2" s="7" t="s">
-        <v>212</v>
+      <c r="BC2" s="22" t="s">
+        <v>282</v>
       </c>
       <c r="BD2">
         <v>92879</v>
@@ -2756,25 +2883,25 @@
       <c r="BT2" s="4">
         <v>20918</v>
       </c>
-      <c r="BU2" s="15" t="s">
+      <c r="BU2" t="s">
         <v>220</v>
       </c>
-      <c r="BV2" s="15" t="s">
+      <c r="BV2" t="s">
         <v>240</v>
       </c>
-      <c r="BW2" s="15" t="s">
+      <c r="BW2" t="s">
         <v>227</v>
       </c>
-      <c r="BX2" s="17" t="s">
+      <c r="BX2" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="BY2" s="23" t="s">
+      <c r="BY2" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="BZ2" s="17" t="s">
+      <c r="BZ2" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="CA2" s="21" t="s">
+      <c r="CA2" s="15" t="s">
         <v>247</v>
       </c>
       <c r="CB2" t="s">
@@ -2843,28 +2970,28 @@
       <c r="CW2">
         <v>2</v>
       </c>
-      <c r="CX2" s="15">
+      <c r="CX2">
         <v>34000</v>
       </c>
-      <c r="CY2" s="19" t="s">
+      <c r="CY2" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="CZ2" s="15" t="s">
+      <c r="CZ2" t="s">
         <v>240</v>
       </c>
-      <c r="DA2" s="15" t="s">
+      <c r="DA2" t="s">
         <v>227</v>
       </c>
-      <c r="DB2" s="17" t="s">
+      <c r="DB2" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="DC2" s="16" t="s">
+      <c r="DC2" t="s">
         <v>247</v>
       </c>
-      <c r="DD2" s="17" t="s">
+      <c r="DD2" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="DE2" s="21" t="s">
+      <c r="DE2" s="15" t="s">
         <v>247</v>
       </c>
       <c r="DF2" t="s">
@@ -2933,176 +3060,92 @@
       <c r="EA2" s="1">
         <v>0</v>
       </c>
-      <c r="EB2" s="20">
+      <c r="EB2" s="17">
         <v>29000</v>
       </c>
-      <c r="EC2" s="15" t="s">
+      <c r="EC2" t="s">
         <v>220</v>
       </c>
-      <c r="ED2" s="15" t="s">
+      <c r="ED2" t="s">
         <v>224</v>
       </c>
-      <c r="EE2" s="15" t="s">
+      <c r="EE2" t="s">
         <v>227</v>
       </c>
-      <c r="EF2" s="17" t="s">
+      <c r="EF2" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="EG2" s="16" t="s">
+      <c r="EG2" t="s">
         <v>247</v>
       </c>
-      <c r="EH2" s="17" t="s">
+      <c r="EH2" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="EI2" s="21" t="s">
+      <c r="EI2" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="EJ2" s="15"/>
-      <c r="EK2" s="15"/>
-      <c r="EL2" s="15"/>
-      <c r="EM2" s="15"/>
-      <c r="EN2" s="15"/>
-      <c r="EO2" s="15"/>
-      <c r="EP2" s="15"/>
-      <c r="EQ2" s="15"/>
-      <c r="ER2" s="15"/>
-      <c r="ES2" s="15"/>
-      <c r="ET2" s="15"/>
-      <c r="EU2" s="15"/>
-      <c r="EV2" s="15"/>
-      <c r="EW2" s="15"/>
-      <c r="EX2" s="15"/>
-      <c r="EY2" s="15"/>
-      <c r="EZ2" s="15"/>
-      <c r="FA2" s="15"/>
-      <c r="FB2" s="15"/>
-      <c r="FC2" s="15"/>
-      <c r="FD2" s="15"/>
-      <c r="FE2" s="15"/>
-      <c r="FF2" s="15"/>
-      <c r="FG2" s="15"/>
-      <c r="FH2" s="15"/>
-      <c r="FI2" s="15"/>
-      <c r="FJ2" s="15"/>
-      <c r="FK2" s="15"/>
-      <c r="FL2" s="15"/>
-      <c r="FM2" s="15"/>
-      <c r="FN2" s="15"/>
-      <c r="FO2" s="15"/>
-      <c r="FP2" s="15"/>
-      <c r="FQ2" s="15"/>
-      <c r="FR2" s="15"/>
-      <c r="FS2" s="15"/>
-      <c r="FT2" s="15"/>
-      <c r="FU2" s="15"/>
-      <c r="FV2" s="15"/>
-      <c r="FW2" s="15"/>
-      <c r="FX2" s="15"/>
-      <c r="FY2" s="15"/>
-      <c r="FZ2" s="15"/>
-      <c r="GA2" s="15"/>
-      <c r="GB2" s="15"/>
-      <c r="GC2" s="15"/>
-      <c r="GD2" s="15"/>
-      <c r="GE2" s="15"/>
-      <c r="GF2" s="15"/>
-      <c r="GG2" s="15"/>
-      <c r="GH2" s="15"/>
-      <c r="GI2" s="15"/>
-      <c r="GJ2" s="15"/>
-      <c r="GK2" s="15"/>
-      <c r="GL2" s="15"/>
-      <c r="GM2" s="15"/>
-      <c r="GN2" s="15"/>
-      <c r="GO2" s="15"/>
-      <c r="GP2" s="15"/>
-      <c r="GQ2" s="15"/>
-      <c r="GR2" s="15"/>
-      <c r="GS2" s="15"/>
-      <c r="GT2" s="15"/>
-      <c r="GU2" s="15"/>
-      <c r="GV2" s="15"/>
-      <c r="GW2" s="15"/>
-      <c r="GX2" s="15"/>
-      <c r="GY2" s="15"/>
-      <c r="GZ2" s="15"/>
-      <c r="HA2" s="15"/>
-      <c r="HB2" s="15"/>
-      <c r="HC2" s="15"/>
-      <c r="HD2" s="15"/>
-      <c r="HE2" s="15"/>
-      <c r="HF2" s="15"/>
-      <c r="HG2" s="15"/>
-      <c r="HH2" s="15"/>
-      <c r="HI2" s="15"/>
-      <c r="HJ2" s="15"/>
-      <c r="HK2" s="15"/>
-      <c r="HL2" s="15"/>
-      <c r="HM2" s="15"/>
-      <c r="HN2" s="15"/>
-      <c r="HO2" s="15"/>
-      <c r="HP2" s="15"/>
-      <c r="HQ2" s="15"/>
-      <c r="HR2" s="15"/>
-      <c r="HS2" s="15"/>
-      <c r="HT2" s="15"/>
-      <c r="HU2" s="15"/>
-      <c r="HV2" s="15"/>
-      <c r="HW2" s="15"/>
-      <c r="HX2" s="15"/>
-      <c r="HY2" s="15"/>
-      <c r="HZ2" s="15"/>
-      <c r="IA2" s="15"/>
-      <c r="IB2" s="15"/>
-      <c r="IC2" s="15"/>
-      <c r="ID2" s="15"/>
-      <c r="IE2" s="15"/>
-      <c r="IF2" s="15"/>
-      <c r="IG2" s="15"/>
-      <c r="IH2" s="15"/>
-      <c r="II2" s="15"/>
-      <c r="IJ2" s="15"/>
-      <c r="IK2" s="15"/>
-      <c r="IL2" s="15"/>
-      <c r="IM2" s="15"/>
-      <c r="IN2" s="15"/>
-      <c r="IO2" s="15"/>
-      <c r="IP2" s="15"/>
-      <c r="IQ2" s="15"/>
-      <c r="IR2" s="15"/>
-      <c r="IS2" s="15"/>
-      <c r="IT2" s="15"/>
-      <c r="IU2" s="15"/>
-      <c r="IV2" s="15"/>
-      <c r="IW2" s="15"/>
-      <c r="IX2" s="15"/>
-      <c r="IY2" s="15"/>
-      <c r="IZ2" s="15"/>
-      <c r="JA2" s="15"/>
-      <c r="JB2" s="15"/>
-      <c r="JC2" s="15"/>
-      <c r="JD2" s="15"/>
-      <c r="JE2" s="15"/>
-      <c r="JF2" s="15"/>
-      <c r="JG2" s="15"/>
-      <c r="JH2" s="15"/>
-      <c r="JI2" s="15"/>
-      <c r="JJ2" s="15"/>
-      <c r="JK2" s="15"/>
-      <c r="JL2" s="15"/>
-      <c r="JM2" s="15"/>
-      <c r="JN2" s="15"/>
-      <c r="JO2" s="15"/>
-      <c r="JP2" s="15"/>
-      <c r="JQ2" s="15"/>
-      <c r="JR2" s="15"/>
-      <c r="JS2" s="15"/>
-      <c r="JT2" s="15"/>
-      <c r="JU2" s="15"/>
-      <c r="JV2" s="15"/>
-      <c r="JW2" s="15"/>
+      <c r="EJ2" t="s">
+        <v>220</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>240</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>227</v>
+      </c>
+      <c r="EM2" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="EN2" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>9</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>269</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>90</v>
+      </c>
+      <c r="ER2">
+        <v>183934904</v>
+      </c>
+      <c r="ES2" t="s">
+        <v>205</v>
+      </c>
+      <c r="ET2">
+        <v>92879</v>
+      </c>
+      <c r="EU2">
+        <v>5</v>
+      </c>
+      <c r="EV2">
+        <v>3</v>
+      </c>
+      <c r="EW2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="EX2">
+        <v>9232003</v>
+      </c>
+      <c r="EY2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="EZ2">
+        <v>1638493959</v>
+      </c>
+      <c r="FA2" s="1">
+        <v>1727838499</v>
+      </c>
+      <c r="FB2" s="1">
+        <v>2893930406</v>
+      </c>
+      <c r="FC2" s="21" t="s">
+        <v>281</v>
+      </c>
     </row>
-    <row r="3" spans="1:283" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:278" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -3229,25 +3272,25 @@
       <c r="AP3" s="4">
         <v>8092014</v>
       </c>
-      <c r="AQ3" s="15" t="s">
+      <c r="AQ3" t="s">
         <v>221</v>
       </c>
-      <c r="AR3" s="15" t="s">
+      <c r="AR3" t="s">
         <v>225</v>
       </c>
-      <c r="AS3" s="15" t="s">
+      <c r="AS3" t="s">
         <v>228</v>
       </c>
-      <c r="AT3" s="17" t="s">
+      <c r="AT3" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="AU3" s="16" t="s">
+      <c r="AU3" t="s">
         <v>247</v>
       </c>
-      <c r="AV3" s="17" t="s">
+      <c r="AV3" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="AW3" s="21" t="s">
+      <c r="AW3" s="15" t="s">
         <v>247</v>
       </c>
       <c r="AX3" t="s">
@@ -3286,13 +3329,13 @@
       <c r="BI3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="BJ3" s="22">
+      <c r="BJ3" s="18">
         <v>9999999999</v>
       </c>
-      <c r="BK3" s="22">
+      <c r="BK3" s="18">
         <v>8888888888</v>
       </c>
-      <c r="BL3" s="22">
+      <c r="BL3" s="18">
         <v>7777777777</v>
       </c>
       <c r="BM3" s="4" t="s">
@@ -3319,206 +3362,41 @@
       <c r="BT3" s="4">
         <v>26500</v>
       </c>
-      <c r="BU3" s="15" t="s">
+      <c r="BU3" t="s">
         <v>221</v>
       </c>
-      <c r="BV3" s="15" t="s">
+      <c r="BV3" t="s">
         <v>225</v>
       </c>
-      <c r="BW3" s="15" t="s">
+      <c r="BW3" t="s">
         <v>228</v>
       </c>
-      <c r="BX3" s="17" t="s">
+      <c r="BX3" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="BY3" s="24" t="s">
+      <c r="BY3" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="BZ3" s="17" t="s">
+      <c r="BZ3" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="CA3" s="21" t="s">
+      <c r="CA3" s="15" t="s">
         <v>246</v>
       </c>
       <c r="CR3" s="5"/>
-      <c r="CX3" s="15"/>
-      <c r="CY3" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="CZ3" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="DA3" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="DB3" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="DC3" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="DD3" s="17" t="s">
-        <v>246</v>
-      </c>
-      <c r="DE3" s="21" t="s">
-        <v>246</v>
-      </c>
+      <c r="CY3" s="5"/>
+      <c r="DB3" s="4"/>
+      <c r="DD3" s="4"/>
+      <c r="DE3" s="15"/>
       <c r="DU3" s="4"/>
-      <c r="DW3" s="15"/>
       <c r="EB3" s="4"/>
-      <c r="EC3" s="15"/>
-      <c r="ED3" s="15"/>
-      <c r="EE3" s="15"/>
-      <c r="EF3" s="17"/>
-      <c r="EG3" s="16"/>
-      <c r="EH3" s="17"/>
-      <c r="EI3" s="18"/>
-      <c r="EJ3" s="15"/>
-      <c r="EK3" s="15"/>
-      <c r="EL3" s="15"/>
-      <c r="EM3" s="15"/>
-      <c r="EN3" s="15"/>
-      <c r="EO3" s="15"/>
-      <c r="EP3" s="15"/>
-      <c r="EQ3" s="15"/>
-      <c r="ER3" s="15"/>
-      <c r="ES3" s="15"/>
-      <c r="ET3" s="15"/>
-      <c r="EU3" s="15"/>
-      <c r="EV3" s="15"/>
-      <c r="EW3" s="15"/>
-      <c r="EX3" s="15"/>
-      <c r="EY3" s="15"/>
-      <c r="EZ3" s="15"/>
-      <c r="FA3" s="15"/>
-      <c r="FB3" s="15"/>
-      <c r="FC3" s="15"/>
-      <c r="FD3" s="15"/>
-      <c r="FE3" s="15"/>
-      <c r="FF3" s="15"/>
-      <c r="FG3" s="15"/>
-      <c r="FH3" s="15"/>
-      <c r="FI3" s="15"/>
-      <c r="FJ3" s="15"/>
-      <c r="FK3" s="15"/>
-      <c r="FL3" s="15"/>
-      <c r="FM3" s="15"/>
-      <c r="FN3" s="15"/>
-      <c r="FO3" s="15"/>
-      <c r="FP3" s="15"/>
-      <c r="FQ3" s="15"/>
-      <c r="FR3" s="15"/>
-      <c r="FS3" s="15"/>
-      <c r="FT3" s="15"/>
-      <c r="FU3" s="15"/>
-      <c r="FV3" s="15"/>
-      <c r="FW3" s="15"/>
-      <c r="FX3" s="15"/>
-      <c r="FY3" s="15"/>
-      <c r="FZ3" s="15"/>
-      <c r="GA3" s="15"/>
-      <c r="GB3" s="15"/>
-      <c r="GC3" s="15"/>
-      <c r="GD3" s="15"/>
-      <c r="GE3" s="15"/>
-      <c r="GF3" s="15"/>
-      <c r="GG3" s="15"/>
-      <c r="GH3" s="15"/>
-      <c r="GI3" s="15"/>
-      <c r="GJ3" s="15"/>
-      <c r="GK3" s="15"/>
-      <c r="GL3" s="15"/>
-      <c r="GM3" s="15"/>
-      <c r="GN3" s="15"/>
-      <c r="GO3" s="15"/>
-      <c r="GP3" s="15"/>
-      <c r="GQ3" s="15"/>
-      <c r="GR3" s="15"/>
-      <c r="GS3" s="15"/>
-      <c r="GT3" s="15"/>
-      <c r="GU3" s="15"/>
-      <c r="GV3" s="15"/>
-      <c r="GW3" s="15"/>
-      <c r="GX3" s="15"/>
-      <c r="GY3" s="15"/>
-      <c r="GZ3" s="15"/>
-      <c r="HA3" s="15"/>
-      <c r="HB3" s="15"/>
-      <c r="HC3" s="15"/>
-      <c r="HD3" s="15"/>
-      <c r="HE3" s="15"/>
-      <c r="HF3" s="15"/>
-      <c r="HG3" s="15"/>
-      <c r="HH3" s="15"/>
-      <c r="HI3" s="15"/>
-      <c r="HJ3" s="15"/>
-      <c r="HK3" s="15"/>
-      <c r="HL3" s="15"/>
-      <c r="HM3" s="15"/>
-      <c r="HN3" s="15"/>
-      <c r="HO3" s="15"/>
-      <c r="HP3" s="15"/>
-      <c r="HQ3" s="15"/>
-      <c r="HR3" s="15"/>
-      <c r="HS3" s="15"/>
-      <c r="HT3" s="15"/>
-      <c r="HU3" s="15"/>
-      <c r="HV3" s="15"/>
-      <c r="HW3" s="15"/>
-      <c r="HX3" s="15"/>
-      <c r="HY3" s="15"/>
-      <c r="HZ3" s="15"/>
-      <c r="IA3" s="15"/>
-      <c r="IB3" s="15"/>
-      <c r="IC3" s="15"/>
-      <c r="ID3" s="15"/>
-      <c r="IE3" s="15"/>
-      <c r="IF3" s="15"/>
-      <c r="IG3" s="15"/>
-      <c r="IH3" s="15"/>
-      <c r="II3" s="15"/>
-      <c r="IJ3" s="15"/>
-      <c r="IK3" s="15"/>
-      <c r="IL3" s="15"/>
-      <c r="IM3" s="15"/>
-      <c r="IN3" s="15"/>
-      <c r="IO3" s="15"/>
-      <c r="IP3" s="15"/>
-      <c r="IQ3" s="15"/>
-      <c r="IR3" s="15"/>
-      <c r="IS3" s="15"/>
-      <c r="IT3" s="15"/>
-      <c r="IU3" s="15"/>
-      <c r="IV3" s="15"/>
-      <c r="IW3" s="15"/>
-      <c r="IX3" s="15"/>
-      <c r="IY3" s="15"/>
-      <c r="IZ3" s="15"/>
-      <c r="JA3" s="15"/>
-      <c r="JB3" s="15"/>
-      <c r="JC3" s="15"/>
-      <c r="JD3" s="15"/>
-      <c r="JE3" s="15"/>
-      <c r="JF3" s="15"/>
-      <c r="JG3" s="15"/>
-      <c r="JH3" s="15"/>
-      <c r="JI3" s="15"/>
-      <c r="JJ3" s="15"/>
-      <c r="JK3" s="15"/>
-      <c r="JL3" s="15"/>
-      <c r="JM3" s="15"/>
-      <c r="JN3" s="15"/>
-      <c r="JO3" s="15"/>
-      <c r="JP3" s="15"/>
-      <c r="JQ3" s="15"/>
-      <c r="JR3" s="15"/>
-      <c r="JS3" s="15"/>
-      <c r="JT3" s="15"/>
-      <c r="JU3" s="15"/>
-      <c r="JV3" s="15"/>
-      <c r="JW3" s="15"/>
+      <c r="EF3" s="4"/>
+      <c r="EH3" s="4"/>
+      <c r="EI3" s="15"/>
+      <c r="EM3" s="4"/>
+      <c r="FC3" s="4"/>
     </row>
-    <row r="4" spans="1:283" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:278" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="C4" s="5"/>
       <c r="S4" s="5"/>
@@ -3527,189 +3405,27 @@
       <c r="AI4" s="4"/>
       <c r="AP4" s="4"/>
       <c r="AT4" s="4"/>
-      <c r="AU4" s="15"/>
       <c r="AV4" s="4"/>
-      <c r="AW4" s="18"/>
-      <c r="BK4" s="15"/>
-      <c r="BL4" s="15"/>
+      <c r="AW4" s="15"/>
       <c r="BM4" s="4"/>
-      <c r="BR4" s="15"/>
-      <c r="BS4" s="15"/>
       <c r="BT4" s="4"/>
-      <c r="BU4" s="15"/>
-      <c r="BV4" s="15"/>
-      <c r="BW4" s="15"/>
       <c r="BX4" s="4"/>
       <c r="BZ4" s="4"/>
-      <c r="CA4" s="18"/>
-      <c r="CN4" s="15"/>
-      <c r="CO4" s="15"/>
+      <c r="CA4" s="15"/>
       <c r="CQ4" s="4"/>
-      <c r="CU4" s="15"/>
-      <c r="CV4" s="15"/>
-      <c r="CW4" s="15"/>
       <c r="CX4" s="4"/>
-      <c r="CZ4" s="15"/>
       <c r="DB4" s="4"/>
       <c r="DD4" s="4"/>
-      <c r="DE4" s="18"/>
-      <c r="DL4" s="15"/>
-      <c r="DQ4" s="15"/>
-      <c r="DS4" s="15"/>
+      <c r="DE4" s="15"/>
       <c r="DU4" s="4"/>
-      <c r="DW4" s="15"/>
-      <c r="DX4" s="15"/>
-      <c r="DY4" s="15"/>
       <c r="EB4" s="4"/>
       <c r="EF4" s="4"/>
       <c r="EH4" s="4"/>
-      <c r="EI4" s="18"/>
-      <c r="EJ4" s="15"/>
-      <c r="EK4" s="15"/>
-      <c r="EL4" s="15"/>
-      <c r="EM4" s="15"/>
-      <c r="EN4" s="15"/>
-      <c r="EO4" s="15"/>
-      <c r="EP4" s="15"/>
-      <c r="EQ4" s="15"/>
-      <c r="ER4" s="15"/>
-      <c r="ES4" s="15"/>
-      <c r="ET4" s="15"/>
-      <c r="EU4" s="15"/>
-      <c r="EV4" s="15"/>
-      <c r="EW4" s="15"/>
-      <c r="EX4" s="15"/>
-      <c r="EY4" s="15"/>
-      <c r="EZ4" s="15"/>
-      <c r="FA4" s="15"/>
-      <c r="FB4" s="15"/>
-      <c r="FC4" s="15"/>
-      <c r="FD4" s="15"/>
-      <c r="FE4" s="15"/>
-      <c r="FF4" s="15"/>
-      <c r="FG4" s="15"/>
-      <c r="FH4" s="15"/>
-      <c r="FI4" s="15"/>
-      <c r="FJ4" s="15"/>
-      <c r="FK4" s="15"/>
-      <c r="FL4" s="15"/>
-      <c r="FM4" s="15"/>
-      <c r="FN4" s="15"/>
-      <c r="FO4" s="15"/>
-      <c r="FP4" s="15"/>
-      <c r="FQ4" s="15"/>
-      <c r="FR4" s="15"/>
-      <c r="FS4" s="15"/>
-      <c r="FT4" s="15"/>
-      <c r="FU4" s="15"/>
-      <c r="FV4" s="15"/>
-      <c r="FW4" s="15"/>
-      <c r="FX4" s="15"/>
-      <c r="FY4" s="15"/>
-      <c r="FZ4" s="15"/>
-      <c r="GA4" s="15"/>
-      <c r="GB4" s="15"/>
-      <c r="GC4" s="15"/>
-      <c r="GD4" s="15"/>
-      <c r="GE4" s="15"/>
-      <c r="GF4" s="15"/>
-      <c r="GG4" s="15"/>
-      <c r="GH4" s="15"/>
-      <c r="GI4" s="15"/>
-      <c r="GJ4" s="15"/>
-      <c r="GK4" s="15"/>
-      <c r="GL4" s="15"/>
-      <c r="GM4" s="15"/>
-      <c r="GN4" s="15"/>
-      <c r="GO4" s="15"/>
-      <c r="GP4" s="15"/>
-      <c r="GQ4" s="15"/>
-      <c r="GR4" s="15"/>
-      <c r="GS4" s="15"/>
-      <c r="GT4" s="15"/>
-      <c r="GU4" s="15"/>
-      <c r="GV4" s="15"/>
-      <c r="GW4" s="15"/>
-      <c r="GX4" s="15"/>
-      <c r="GY4" s="15"/>
-      <c r="GZ4" s="15"/>
-      <c r="HA4" s="15"/>
-      <c r="HB4" s="15"/>
-      <c r="HC4" s="15"/>
-      <c r="HD4" s="15"/>
-      <c r="HE4" s="15"/>
-      <c r="HF4" s="15"/>
-      <c r="HG4" s="15"/>
-      <c r="HH4" s="15"/>
-      <c r="HI4" s="15"/>
-      <c r="HJ4" s="15"/>
-      <c r="HK4" s="15"/>
-      <c r="HL4" s="15"/>
-      <c r="HM4" s="15"/>
-      <c r="HN4" s="15"/>
-      <c r="HO4" s="15"/>
-      <c r="HP4" s="15"/>
-      <c r="HQ4" s="15"/>
-      <c r="HR4" s="15"/>
-      <c r="HS4" s="15"/>
-      <c r="HT4" s="15"/>
-      <c r="HU4" s="15"/>
-      <c r="HV4" s="15"/>
-      <c r="HW4" s="15"/>
-      <c r="HX4" s="15"/>
-      <c r="HY4" s="15"/>
-      <c r="HZ4" s="15"/>
-      <c r="IA4" s="15"/>
-      <c r="IB4" s="15"/>
-      <c r="IC4" s="15"/>
-      <c r="ID4" s="15"/>
-      <c r="IE4" s="15"/>
-      <c r="IF4" s="15"/>
-      <c r="IG4" s="15"/>
-      <c r="IH4" s="15"/>
-      <c r="II4" s="15"/>
-      <c r="IJ4" s="15"/>
-      <c r="IK4" s="15"/>
-      <c r="IL4" s="15"/>
-      <c r="IM4" s="15"/>
-      <c r="IN4" s="15"/>
-      <c r="IO4" s="15"/>
-      <c r="IP4" s="15"/>
-      <c r="IQ4" s="15"/>
-      <c r="IR4" s="15"/>
-      <c r="IS4" s="15"/>
-      <c r="IT4" s="15"/>
-      <c r="IU4" s="15"/>
-      <c r="IV4" s="15"/>
-      <c r="IW4" s="15"/>
-      <c r="IX4" s="15"/>
-      <c r="IY4" s="15"/>
-      <c r="IZ4" s="15"/>
-      <c r="JA4" s="15"/>
-      <c r="JB4" s="15"/>
-      <c r="JC4" s="15"/>
-      <c r="JD4" s="15"/>
-      <c r="JE4" s="15"/>
-      <c r="JF4" s="15"/>
-      <c r="JG4" s="15"/>
-      <c r="JH4" s="15"/>
-      <c r="JI4" s="15"/>
-      <c r="JJ4" s="15"/>
-      <c r="JK4" s="15"/>
-      <c r="JL4" s="15"/>
-      <c r="JM4" s="15"/>
-      <c r="JN4" s="15"/>
-      <c r="JO4" s="15"/>
-      <c r="JP4" s="15"/>
-      <c r="JQ4" s="15"/>
-      <c r="JR4" s="15"/>
-      <c r="JS4" s="15"/>
-      <c r="JT4" s="15"/>
-      <c r="JU4" s="15"/>
-      <c r="JV4" s="15"/>
-      <c r="JW4" s="15"/>
+      <c r="EI4" s="15"/>
+      <c r="EM4" s="4"/>
+      <c r="FC4" s="4"/>
     </row>
-    <row r="5" spans="1:283" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:278" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="C5" s="5"/>
       <c r="S5" s="5"/>
@@ -3718,189 +3434,27 @@
       <c r="AI5" s="4"/>
       <c r="AP5" s="4"/>
       <c r="AT5" s="4"/>
-      <c r="AU5" s="15"/>
       <c r="AV5" s="4"/>
-      <c r="AW5" s="18"/>
-      <c r="BK5" s="15"/>
-      <c r="BL5" s="15"/>
+      <c r="AW5" s="15"/>
       <c r="BM5" s="4"/>
-      <c r="BR5" s="15"/>
-      <c r="BS5" s="15"/>
       <c r="BT5" s="4"/>
-      <c r="BU5" s="15"/>
-      <c r="BV5" s="15"/>
-      <c r="BW5" s="15"/>
       <c r="BX5" s="4"/>
       <c r="BZ5" s="4"/>
-      <c r="CA5" s="18"/>
-      <c r="CN5" s="15"/>
-      <c r="CO5" s="15"/>
+      <c r="CA5" s="15"/>
       <c r="CQ5" s="4"/>
-      <c r="CU5" s="15"/>
-      <c r="CV5" s="15"/>
-      <c r="CW5" s="15"/>
       <c r="CX5" s="4"/>
-      <c r="CZ5" s="15"/>
       <c r="DB5" s="4"/>
       <c r="DD5" s="4"/>
-      <c r="DE5" s="18"/>
-      <c r="DL5" s="15"/>
-      <c r="DQ5" s="15"/>
-      <c r="DS5" s="15"/>
+      <c r="DE5" s="15"/>
       <c r="DU5" s="4"/>
-      <c r="DW5" s="15"/>
-      <c r="DX5" s="15"/>
-      <c r="DY5" s="15"/>
       <c r="EB5" s="4"/>
       <c r="EF5" s="4"/>
       <c r="EH5" s="4"/>
-      <c r="EI5" s="18"/>
-      <c r="EJ5" s="15"/>
-      <c r="EK5" s="15"/>
-      <c r="EL5" s="15"/>
-      <c r="EM5" s="15"/>
-      <c r="EN5" s="15"/>
-      <c r="EO5" s="15"/>
-      <c r="EP5" s="15"/>
-      <c r="EQ5" s="15"/>
-      <c r="ER5" s="15"/>
-      <c r="ES5" s="15"/>
-      <c r="ET5" s="15"/>
-      <c r="EU5" s="15"/>
-      <c r="EV5" s="15"/>
-      <c r="EW5" s="15"/>
-      <c r="EX5" s="15"/>
-      <c r="EY5" s="15"/>
-      <c r="EZ5" s="15"/>
-      <c r="FA5" s="15"/>
-      <c r="FB5" s="15"/>
-      <c r="FC5" s="15"/>
-      <c r="FD5" s="15"/>
-      <c r="FE5" s="15"/>
-      <c r="FF5" s="15"/>
-      <c r="FG5" s="15"/>
-      <c r="FH5" s="15"/>
-      <c r="FI5" s="15"/>
-      <c r="FJ5" s="15"/>
-      <c r="FK5" s="15"/>
-      <c r="FL5" s="15"/>
-      <c r="FM5" s="15"/>
-      <c r="FN5" s="15"/>
-      <c r="FO5" s="15"/>
-      <c r="FP5" s="15"/>
-      <c r="FQ5" s="15"/>
-      <c r="FR5" s="15"/>
-      <c r="FS5" s="15"/>
-      <c r="FT5" s="15"/>
-      <c r="FU5" s="15"/>
-      <c r="FV5" s="15"/>
-      <c r="FW5" s="15"/>
-      <c r="FX5" s="15"/>
-      <c r="FY5" s="15"/>
-      <c r="FZ5" s="15"/>
-      <c r="GA5" s="15"/>
-      <c r="GB5" s="15"/>
-      <c r="GC5" s="15"/>
-      <c r="GD5" s="15"/>
-      <c r="GE5" s="15"/>
-      <c r="GF5" s="15"/>
-      <c r="GG5" s="15"/>
-      <c r="GH5" s="15"/>
-      <c r="GI5" s="15"/>
-      <c r="GJ5" s="15"/>
-      <c r="GK5" s="15"/>
-      <c r="GL5" s="15"/>
-      <c r="GM5" s="15"/>
-      <c r="GN5" s="15"/>
-      <c r="GO5" s="15"/>
-      <c r="GP5" s="15"/>
-      <c r="GQ5" s="15"/>
-      <c r="GR5" s="15"/>
-      <c r="GS5" s="15"/>
-      <c r="GT5" s="15"/>
-      <c r="GU5" s="15"/>
-      <c r="GV5" s="15"/>
-      <c r="GW5" s="15"/>
-      <c r="GX5" s="15"/>
-      <c r="GY5" s="15"/>
-      <c r="GZ5" s="15"/>
-      <c r="HA5" s="15"/>
-      <c r="HB5" s="15"/>
-      <c r="HC5" s="15"/>
-      <c r="HD5" s="15"/>
-      <c r="HE5" s="15"/>
-      <c r="HF5" s="15"/>
-      <c r="HG5" s="15"/>
-      <c r="HH5" s="15"/>
-      <c r="HI5" s="15"/>
-      <c r="HJ5" s="15"/>
-      <c r="HK5" s="15"/>
-      <c r="HL5" s="15"/>
-      <c r="HM5" s="15"/>
-      <c r="HN5" s="15"/>
-      <c r="HO5" s="15"/>
-      <c r="HP5" s="15"/>
-      <c r="HQ5" s="15"/>
-      <c r="HR5" s="15"/>
-      <c r="HS5" s="15"/>
-      <c r="HT5" s="15"/>
-      <c r="HU5" s="15"/>
-      <c r="HV5" s="15"/>
-      <c r="HW5" s="15"/>
-      <c r="HX5" s="15"/>
-      <c r="HY5" s="15"/>
-      <c r="HZ5" s="15"/>
-      <c r="IA5" s="15"/>
-      <c r="IB5" s="15"/>
-      <c r="IC5" s="15"/>
-      <c r="ID5" s="15"/>
-      <c r="IE5" s="15"/>
-      <c r="IF5" s="15"/>
-      <c r="IG5" s="15"/>
-      <c r="IH5" s="15"/>
-      <c r="II5" s="15"/>
-      <c r="IJ5" s="15"/>
-      <c r="IK5" s="15"/>
-      <c r="IL5" s="15"/>
-      <c r="IM5" s="15"/>
-      <c r="IN5" s="15"/>
-      <c r="IO5" s="15"/>
-      <c r="IP5" s="15"/>
-      <c r="IQ5" s="15"/>
-      <c r="IR5" s="15"/>
-      <c r="IS5" s="15"/>
-      <c r="IT5" s="15"/>
-      <c r="IU5" s="15"/>
-      <c r="IV5" s="15"/>
-      <c r="IW5" s="15"/>
-      <c r="IX5" s="15"/>
-      <c r="IY5" s="15"/>
-      <c r="IZ5" s="15"/>
-      <c r="JA5" s="15"/>
-      <c r="JB5" s="15"/>
-      <c r="JC5" s="15"/>
-      <c r="JD5" s="15"/>
-      <c r="JE5" s="15"/>
-      <c r="JF5" s="15"/>
-      <c r="JG5" s="15"/>
-      <c r="JH5" s="15"/>
-      <c r="JI5" s="15"/>
-      <c r="JJ5" s="15"/>
-      <c r="JK5" s="15"/>
-      <c r="JL5" s="15"/>
-      <c r="JM5" s="15"/>
-      <c r="JN5" s="15"/>
-      <c r="JO5" s="15"/>
-      <c r="JP5" s="15"/>
-      <c r="JQ5" s="15"/>
-      <c r="JR5" s="15"/>
-      <c r="JS5" s="15"/>
-      <c r="JT5" s="15"/>
-      <c r="JU5" s="15"/>
-      <c r="JV5" s="15"/>
-      <c r="JW5" s="15"/>
+      <c r="EI5" s="15"/>
+      <c r="EM5" s="4"/>
+      <c r="FC5" s="4"/>
     </row>
-    <row r="6" spans="1:283" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:278" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="C6" s="5"/>
       <c r="S6" s="5"/>
@@ -3909,189 +3463,27 @@
       <c r="AI6" s="4"/>
       <c r="AP6" s="4"/>
       <c r="AT6" s="4"/>
-      <c r="AU6" s="15"/>
       <c r="AV6" s="4"/>
-      <c r="AW6" s="18"/>
-      <c r="BK6" s="15"/>
-      <c r="BL6" s="15"/>
+      <c r="AW6" s="15"/>
       <c r="BM6" s="4"/>
-      <c r="BR6" s="15"/>
-      <c r="BS6" s="15"/>
       <c r="BT6" s="4"/>
-      <c r="BU6" s="15"/>
-      <c r="BV6" s="15"/>
-      <c r="BW6" s="15"/>
       <c r="BX6" s="4"/>
       <c r="BZ6" s="4"/>
-      <c r="CA6" s="18"/>
-      <c r="CN6" s="15"/>
-      <c r="CO6" s="15"/>
+      <c r="CA6" s="15"/>
       <c r="CQ6" s="4"/>
-      <c r="CU6" s="15"/>
-      <c r="CV6" s="15"/>
-      <c r="CW6" s="15"/>
       <c r="CX6" s="4"/>
-      <c r="CZ6" s="15"/>
       <c r="DB6" s="4"/>
       <c r="DD6" s="4"/>
-      <c r="DE6" s="18"/>
-      <c r="DL6" s="15"/>
-      <c r="DQ6" s="15"/>
-      <c r="DS6" s="15"/>
+      <c r="DE6" s="15"/>
       <c r="DU6" s="4"/>
-      <c r="DW6" s="15"/>
-      <c r="DX6" s="15"/>
-      <c r="DY6" s="15"/>
       <c r="EB6" s="4"/>
       <c r="EF6" s="4"/>
       <c r="EH6" s="4"/>
-      <c r="EI6" s="18"/>
-      <c r="EJ6" s="15"/>
-      <c r="EK6" s="15"/>
-      <c r="EL6" s="15"/>
-      <c r="EM6" s="15"/>
-      <c r="EN6" s="15"/>
-      <c r="EO6" s="15"/>
-      <c r="EP6" s="15"/>
-      <c r="EQ6" s="15"/>
-      <c r="ER6" s="15"/>
-      <c r="ES6" s="15"/>
-      <c r="ET6" s="15"/>
-      <c r="EU6" s="15"/>
-      <c r="EV6" s="15"/>
-      <c r="EW6" s="15"/>
-      <c r="EX6" s="15"/>
-      <c r="EY6" s="15"/>
-      <c r="EZ6" s="15"/>
-      <c r="FA6" s="15"/>
-      <c r="FB6" s="15"/>
-      <c r="FC6" s="15"/>
-      <c r="FD6" s="15"/>
-      <c r="FE6" s="15"/>
-      <c r="FF6" s="15"/>
-      <c r="FG6" s="15"/>
-      <c r="FH6" s="15"/>
-      <c r="FI6" s="15"/>
-      <c r="FJ6" s="15"/>
-      <c r="FK6" s="15"/>
-      <c r="FL6" s="15"/>
-      <c r="FM6" s="15"/>
-      <c r="FN6" s="15"/>
-      <c r="FO6" s="15"/>
-      <c r="FP6" s="15"/>
-      <c r="FQ6" s="15"/>
-      <c r="FR6" s="15"/>
-      <c r="FS6" s="15"/>
-      <c r="FT6" s="15"/>
-      <c r="FU6" s="15"/>
-      <c r="FV6" s="15"/>
-      <c r="FW6" s="15"/>
-      <c r="FX6" s="15"/>
-      <c r="FY6" s="15"/>
-      <c r="FZ6" s="15"/>
-      <c r="GA6" s="15"/>
-      <c r="GB6" s="15"/>
-      <c r="GC6" s="15"/>
-      <c r="GD6" s="15"/>
-      <c r="GE6" s="15"/>
-      <c r="GF6" s="15"/>
-      <c r="GG6" s="15"/>
-      <c r="GH6" s="15"/>
-      <c r="GI6" s="15"/>
-      <c r="GJ6" s="15"/>
-      <c r="GK6" s="15"/>
-      <c r="GL6" s="15"/>
-      <c r="GM6" s="15"/>
-      <c r="GN6" s="15"/>
-      <c r="GO6" s="15"/>
-      <c r="GP6" s="15"/>
-      <c r="GQ6" s="15"/>
-      <c r="GR6" s="15"/>
-      <c r="GS6" s="15"/>
-      <c r="GT6" s="15"/>
-      <c r="GU6" s="15"/>
-      <c r="GV6" s="15"/>
-      <c r="GW6" s="15"/>
-      <c r="GX6" s="15"/>
-      <c r="GY6" s="15"/>
-      <c r="GZ6" s="15"/>
-      <c r="HA6" s="15"/>
-      <c r="HB6" s="15"/>
-      <c r="HC6" s="15"/>
-      <c r="HD6" s="15"/>
-      <c r="HE6" s="15"/>
-      <c r="HF6" s="15"/>
-      <c r="HG6" s="15"/>
-      <c r="HH6" s="15"/>
-      <c r="HI6" s="15"/>
-      <c r="HJ6" s="15"/>
-      <c r="HK6" s="15"/>
-      <c r="HL6" s="15"/>
-      <c r="HM6" s="15"/>
-      <c r="HN6" s="15"/>
-      <c r="HO6" s="15"/>
-      <c r="HP6" s="15"/>
-      <c r="HQ6" s="15"/>
-      <c r="HR6" s="15"/>
-      <c r="HS6" s="15"/>
-      <c r="HT6" s="15"/>
-      <c r="HU6" s="15"/>
-      <c r="HV6" s="15"/>
-      <c r="HW6" s="15"/>
-      <c r="HX6" s="15"/>
-      <c r="HY6" s="15"/>
-      <c r="HZ6" s="15"/>
-      <c r="IA6" s="15"/>
-      <c r="IB6" s="15"/>
-      <c r="IC6" s="15"/>
-      <c r="ID6" s="15"/>
-      <c r="IE6" s="15"/>
-      <c r="IF6" s="15"/>
-      <c r="IG6" s="15"/>
-      <c r="IH6" s="15"/>
-      <c r="II6" s="15"/>
-      <c r="IJ6" s="15"/>
-      <c r="IK6" s="15"/>
-      <c r="IL6" s="15"/>
-      <c r="IM6" s="15"/>
-      <c r="IN6" s="15"/>
-      <c r="IO6" s="15"/>
-      <c r="IP6" s="15"/>
-      <c r="IQ6" s="15"/>
-      <c r="IR6" s="15"/>
-      <c r="IS6" s="15"/>
-      <c r="IT6" s="15"/>
-      <c r="IU6" s="15"/>
-      <c r="IV6" s="15"/>
-      <c r="IW6" s="15"/>
-      <c r="IX6" s="15"/>
-      <c r="IY6" s="15"/>
-      <c r="IZ6" s="15"/>
-      <c r="JA6" s="15"/>
-      <c r="JB6" s="15"/>
-      <c r="JC6" s="15"/>
-      <c r="JD6" s="15"/>
-      <c r="JE6" s="15"/>
-      <c r="JF6" s="15"/>
-      <c r="JG6" s="15"/>
-      <c r="JH6" s="15"/>
-      <c r="JI6" s="15"/>
-      <c r="JJ6" s="15"/>
-      <c r="JK6" s="15"/>
-      <c r="JL6" s="15"/>
-      <c r="JM6" s="15"/>
-      <c r="JN6" s="15"/>
-      <c r="JO6" s="15"/>
-      <c r="JP6" s="15"/>
-      <c r="JQ6" s="15"/>
-      <c r="JR6" s="15"/>
-      <c r="JS6" s="15"/>
-      <c r="JT6" s="15"/>
-      <c r="JU6" s="15"/>
-      <c r="JV6" s="15"/>
-      <c r="JW6" s="15"/>
+      <c r="EI6" s="15"/>
+      <c r="EM6" s="4"/>
+      <c r="FC6" s="4"/>
     </row>
-    <row r="7" spans="1:283" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:278" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="C7" s="5"/>
       <c r="S7" s="5"/>
@@ -4100,189 +3492,27 @@
       <c r="AI7" s="4"/>
       <c r="AP7" s="4"/>
       <c r="AT7" s="4"/>
-      <c r="AU7" s="15"/>
       <c r="AV7" s="4"/>
-      <c r="AW7" s="18"/>
-      <c r="BK7" s="15"/>
-      <c r="BL7" s="15"/>
+      <c r="AW7" s="15"/>
       <c r="BM7" s="4"/>
-      <c r="BR7" s="15"/>
-      <c r="BS7" s="15"/>
       <c r="BT7" s="4"/>
-      <c r="BU7" s="15"/>
-      <c r="BV7" s="15"/>
-      <c r="BW7" s="15"/>
       <c r="BX7" s="4"/>
       <c r="BZ7" s="4"/>
-      <c r="CA7" s="18"/>
-      <c r="CN7" s="15"/>
-      <c r="CO7" s="15"/>
+      <c r="CA7" s="15"/>
       <c r="CQ7" s="4"/>
-      <c r="CU7" s="15"/>
-      <c r="CV7" s="15"/>
-      <c r="CW7" s="15"/>
       <c r="CX7" s="4"/>
-      <c r="CZ7" s="15"/>
       <c r="DB7" s="4"/>
       <c r="DD7" s="4"/>
-      <c r="DE7" s="18"/>
-      <c r="DL7" s="15"/>
-      <c r="DQ7" s="15"/>
-      <c r="DS7" s="15"/>
+      <c r="DE7" s="15"/>
       <c r="DU7" s="4"/>
-      <c r="DW7" s="15"/>
-      <c r="DX7" s="15"/>
-      <c r="DY7" s="15"/>
       <c r="EB7" s="4"/>
       <c r="EF7" s="4"/>
       <c r="EH7" s="4"/>
-      <c r="EI7" s="18"/>
-      <c r="EJ7" s="15"/>
-      <c r="EK7" s="15"/>
-      <c r="EL7" s="15"/>
-      <c r="EM7" s="15"/>
-      <c r="EN7" s="15"/>
-      <c r="EO7" s="15"/>
-      <c r="EP7" s="15"/>
-      <c r="EQ7" s="15"/>
-      <c r="ER7" s="15"/>
-      <c r="ES7" s="15"/>
-      <c r="ET7" s="15"/>
-      <c r="EU7" s="15"/>
-      <c r="EV7" s="15"/>
-      <c r="EW7" s="15"/>
-      <c r="EX7" s="15"/>
-      <c r="EY7" s="15"/>
-      <c r="EZ7" s="15"/>
-      <c r="FA7" s="15"/>
-      <c r="FB7" s="15"/>
-      <c r="FC7" s="15"/>
-      <c r="FD7" s="15"/>
-      <c r="FE7" s="15"/>
-      <c r="FF7" s="15"/>
-      <c r="FG7" s="15"/>
-      <c r="FH7" s="15"/>
-      <c r="FI7" s="15"/>
-      <c r="FJ7" s="15"/>
-      <c r="FK7" s="15"/>
-      <c r="FL7" s="15"/>
-      <c r="FM7" s="15"/>
-      <c r="FN7" s="15"/>
-      <c r="FO7" s="15"/>
-      <c r="FP7" s="15"/>
-      <c r="FQ7" s="15"/>
-      <c r="FR7" s="15"/>
-      <c r="FS7" s="15"/>
-      <c r="FT7" s="15"/>
-      <c r="FU7" s="15"/>
-      <c r="FV7" s="15"/>
-      <c r="FW7" s="15"/>
-      <c r="FX7" s="15"/>
-      <c r="FY7" s="15"/>
-      <c r="FZ7" s="15"/>
-      <c r="GA7" s="15"/>
-      <c r="GB7" s="15"/>
-      <c r="GC7" s="15"/>
-      <c r="GD7" s="15"/>
-      <c r="GE7" s="15"/>
-      <c r="GF7" s="15"/>
-      <c r="GG7" s="15"/>
-      <c r="GH7" s="15"/>
-      <c r="GI7" s="15"/>
-      <c r="GJ7" s="15"/>
-      <c r="GK7" s="15"/>
-      <c r="GL7" s="15"/>
-      <c r="GM7" s="15"/>
-      <c r="GN7" s="15"/>
-      <c r="GO7" s="15"/>
-      <c r="GP7" s="15"/>
-      <c r="GQ7" s="15"/>
-      <c r="GR7" s="15"/>
-      <c r="GS7" s="15"/>
-      <c r="GT7" s="15"/>
-      <c r="GU7" s="15"/>
-      <c r="GV7" s="15"/>
-      <c r="GW7" s="15"/>
-      <c r="GX7" s="15"/>
-      <c r="GY7" s="15"/>
-      <c r="GZ7" s="15"/>
-      <c r="HA7" s="15"/>
-      <c r="HB7" s="15"/>
-      <c r="HC7" s="15"/>
-      <c r="HD7" s="15"/>
-      <c r="HE7" s="15"/>
-      <c r="HF7" s="15"/>
-      <c r="HG7" s="15"/>
-      <c r="HH7" s="15"/>
-      <c r="HI7" s="15"/>
-      <c r="HJ7" s="15"/>
-      <c r="HK7" s="15"/>
-      <c r="HL7" s="15"/>
-      <c r="HM7" s="15"/>
-      <c r="HN7" s="15"/>
-      <c r="HO7" s="15"/>
-      <c r="HP7" s="15"/>
-      <c r="HQ7" s="15"/>
-      <c r="HR7" s="15"/>
-      <c r="HS7" s="15"/>
-      <c r="HT7" s="15"/>
-      <c r="HU7" s="15"/>
-      <c r="HV7" s="15"/>
-      <c r="HW7" s="15"/>
-      <c r="HX7" s="15"/>
-      <c r="HY7" s="15"/>
-      <c r="HZ7" s="15"/>
-      <c r="IA7" s="15"/>
-      <c r="IB7" s="15"/>
-      <c r="IC7" s="15"/>
-      <c r="ID7" s="15"/>
-      <c r="IE7" s="15"/>
-      <c r="IF7" s="15"/>
-      <c r="IG7" s="15"/>
-      <c r="IH7" s="15"/>
-      <c r="II7" s="15"/>
-      <c r="IJ7" s="15"/>
-      <c r="IK7" s="15"/>
-      <c r="IL7" s="15"/>
-      <c r="IM7" s="15"/>
-      <c r="IN7" s="15"/>
-      <c r="IO7" s="15"/>
-      <c r="IP7" s="15"/>
-      <c r="IQ7" s="15"/>
-      <c r="IR7" s="15"/>
-      <c r="IS7" s="15"/>
-      <c r="IT7" s="15"/>
-      <c r="IU7" s="15"/>
-      <c r="IV7" s="15"/>
-      <c r="IW7" s="15"/>
-      <c r="IX7" s="15"/>
-      <c r="IY7" s="15"/>
-      <c r="IZ7" s="15"/>
-      <c r="JA7" s="15"/>
-      <c r="JB7" s="15"/>
-      <c r="JC7" s="15"/>
-      <c r="JD7" s="15"/>
-      <c r="JE7" s="15"/>
-      <c r="JF7" s="15"/>
-      <c r="JG7" s="15"/>
-      <c r="JH7" s="15"/>
-      <c r="JI7" s="15"/>
-      <c r="JJ7" s="15"/>
-      <c r="JK7" s="15"/>
-      <c r="JL7" s="15"/>
-      <c r="JM7" s="15"/>
-      <c r="JN7" s="15"/>
-      <c r="JO7" s="15"/>
-      <c r="JP7" s="15"/>
-      <c r="JQ7" s="15"/>
-      <c r="JR7" s="15"/>
-      <c r="JS7" s="15"/>
-      <c r="JT7" s="15"/>
-      <c r="JU7" s="15"/>
-      <c r="JV7" s="15"/>
-      <c r="JW7" s="15"/>
+      <c r="EI7" s="15"/>
+      <c r="EM7" s="4"/>
+      <c r="FC7" s="4"/>
     </row>
-    <row r="8" spans="1:283" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:278" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="C8" s="5"/>
       <c r="S8" s="5"/>
@@ -4291,189 +3521,27 @@
       <c r="AI8" s="4"/>
       <c r="AP8" s="4"/>
       <c r="AT8" s="4"/>
-      <c r="AU8" s="15"/>
       <c r="AV8" s="4"/>
-      <c r="AW8" s="18"/>
-      <c r="BK8" s="15"/>
-      <c r="BL8" s="15"/>
+      <c r="AW8" s="15"/>
       <c r="BM8" s="4"/>
-      <c r="BR8" s="15"/>
-      <c r="BS8" s="15"/>
       <c r="BT8" s="4"/>
-      <c r="BU8" s="15"/>
-      <c r="BV8" s="15"/>
-      <c r="BW8" s="15"/>
       <c r="BX8" s="4"/>
       <c r="BZ8" s="4"/>
-      <c r="CA8" s="18"/>
-      <c r="CN8" s="15"/>
-      <c r="CO8" s="15"/>
+      <c r="CA8" s="15"/>
       <c r="CQ8" s="4"/>
-      <c r="CU8" s="15"/>
-      <c r="CV8" s="15"/>
-      <c r="CW8" s="15"/>
       <c r="CX8" s="4"/>
-      <c r="CZ8" s="15"/>
       <c r="DB8" s="4"/>
       <c r="DD8" s="4"/>
-      <c r="DE8" s="18"/>
-      <c r="DL8" s="15"/>
-      <c r="DQ8" s="15"/>
-      <c r="DS8" s="15"/>
+      <c r="DE8" s="15"/>
       <c r="DU8" s="4"/>
-      <c r="DW8" s="15"/>
-      <c r="DX8" s="15"/>
-      <c r="DY8" s="15"/>
       <c r="EB8" s="4"/>
       <c r="EF8" s="4"/>
       <c r="EH8" s="4"/>
-      <c r="EI8" s="18"/>
-      <c r="EJ8" s="15"/>
-      <c r="EK8" s="15"/>
-      <c r="EL8" s="15"/>
-      <c r="EM8" s="15"/>
-      <c r="EN8" s="15"/>
-      <c r="EO8" s="15"/>
-      <c r="EP8" s="15"/>
-      <c r="EQ8" s="15"/>
-      <c r="ER8" s="15"/>
-      <c r="ES8" s="15"/>
-      <c r="ET8" s="15"/>
-      <c r="EU8" s="15"/>
-      <c r="EV8" s="15"/>
-      <c r="EW8" s="15"/>
-      <c r="EX8" s="15"/>
-      <c r="EY8" s="15"/>
-      <c r="EZ8" s="15"/>
-      <c r="FA8" s="15"/>
-      <c r="FB8" s="15"/>
-      <c r="FC8" s="15"/>
-      <c r="FD8" s="15"/>
-      <c r="FE8" s="15"/>
-      <c r="FF8" s="15"/>
-      <c r="FG8" s="15"/>
-      <c r="FH8" s="15"/>
-      <c r="FI8" s="15"/>
-      <c r="FJ8" s="15"/>
-      <c r="FK8" s="15"/>
-      <c r="FL8" s="15"/>
-      <c r="FM8" s="15"/>
-      <c r="FN8" s="15"/>
-      <c r="FO8" s="15"/>
-      <c r="FP8" s="15"/>
-      <c r="FQ8" s="15"/>
-      <c r="FR8" s="15"/>
-      <c r="FS8" s="15"/>
-      <c r="FT8" s="15"/>
-      <c r="FU8" s="15"/>
-      <c r="FV8" s="15"/>
-      <c r="FW8" s="15"/>
-      <c r="FX8" s="15"/>
-      <c r="FY8" s="15"/>
-      <c r="FZ8" s="15"/>
-      <c r="GA8" s="15"/>
-      <c r="GB8" s="15"/>
-      <c r="GC8" s="15"/>
-      <c r="GD8" s="15"/>
-      <c r="GE8" s="15"/>
-      <c r="GF8" s="15"/>
-      <c r="GG8" s="15"/>
-      <c r="GH8" s="15"/>
-      <c r="GI8" s="15"/>
-      <c r="GJ8" s="15"/>
-      <c r="GK8" s="15"/>
-      <c r="GL8" s="15"/>
-      <c r="GM8" s="15"/>
-      <c r="GN8" s="15"/>
-      <c r="GO8" s="15"/>
-      <c r="GP8" s="15"/>
-      <c r="GQ8" s="15"/>
-      <c r="GR8" s="15"/>
-      <c r="GS8" s="15"/>
-      <c r="GT8" s="15"/>
-      <c r="GU8" s="15"/>
-      <c r="GV8" s="15"/>
-      <c r="GW8" s="15"/>
-      <c r="GX8" s="15"/>
-      <c r="GY8" s="15"/>
-      <c r="GZ8" s="15"/>
-      <c r="HA8" s="15"/>
-      <c r="HB8" s="15"/>
-      <c r="HC8" s="15"/>
-      <c r="HD8" s="15"/>
-      <c r="HE8" s="15"/>
-      <c r="HF8" s="15"/>
-      <c r="HG8" s="15"/>
-      <c r="HH8" s="15"/>
-      <c r="HI8" s="15"/>
-      <c r="HJ8" s="15"/>
-      <c r="HK8" s="15"/>
-      <c r="HL8" s="15"/>
-      <c r="HM8" s="15"/>
-      <c r="HN8" s="15"/>
-      <c r="HO8" s="15"/>
-      <c r="HP8" s="15"/>
-      <c r="HQ8" s="15"/>
-      <c r="HR8" s="15"/>
-      <c r="HS8" s="15"/>
-      <c r="HT8" s="15"/>
-      <c r="HU8" s="15"/>
-      <c r="HV8" s="15"/>
-      <c r="HW8" s="15"/>
-      <c r="HX8" s="15"/>
-      <c r="HY8" s="15"/>
-      <c r="HZ8" s="15"/>
-      <c r="IA8" s="15"/>
-      <c r="IB8" s="15"/>
-      <c r="IC8" s="15"/>
-      <c r="ID8" s="15"/>
-      <c r="IE8" s="15"/>
-      <c r="IF8" s="15"/>
-      <c r="IG8" s="15"/>
-      <c r="IH8" s="15"/>
-      <c r="II8" s="15"/>
-      <c r="IJ8" s="15"/>
-      <c r="IK8" s="15"/>
-      <c r="IL8" s="15"/>
-      <c r="IM8" s="15"/>
-      <c r="IN8" s="15"/>
-      <c r="IO8" s="15"/>
-      <c r="IP8" s="15"/>
-      <c r="IQ8" s="15"/>
-      <c r="IR8" s="15"/>
-      <c r="IS8" s="15"/>
-      <c r="IT8" s="15"/>
-      <c r="IU8" s="15"/>
-      <c r="IV8" s="15"/>
-      <c r="IW8" s="15"/>
-      <c r="IX8" s="15"/>
-      <c r="IY8" s="15"/>
-      <c r="IZ8" s="15"/>
-      <c r="JA8" s="15"/>
-      <c r="JB8" s="15"/>
-      <c r="JC8" s="15"/>
-      <c r="JD8" s="15"/>
-      <c r="JE8" s="15"/>
-      <c r="JF8" s="15"/>
-      <c r="JG8" s="15"/>
-      <c r="JH8" s="15"/>
-      <c r="JI8" s="15"/>
-      <c r="JJ8" s="15"/>
-      <c r="JK8" s="15"/>
-      <c r="JL8" s="15"/>
-      <c r="JM8" s="15"/>
-      <c r="JN8" s="15"/>
-      <c r="JO8" s="15"/>
-      <c r="JP8" s="15"/>
-      <c r="JQ8" s="15"/>
-      <c r="JR8" s="15"/>
-      <c r="JS8" s="15"/>
-      <c r="JT8" s="15"/>
-      <c r="JU8" s="15"/>
-      <c r="JV8" s="15"/>
-      <c r="JW8" s="15"/>
+      <c r="EI8" s="15"/>
+      <c r="EM8" s="4"/>
+      <c r="FC8" s="4"/>
     </row>
-    <row r="9" spans="1:283" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:278" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="C9" s="5"/>
       <c r="S9" s="5"/>
@@ -4482,189 +3550,45 @@
       <c r="AI9" s="4"/>
       <c r="AP9" s="4"/>
       <c r="AT9" s="4"/>
-      <c r="AU9" s="15"/>
       <c r="AV9" s="4"/>
-      <c r="AW9" s="18"/>
-      <c r="BK9" s="15"/>
-      <c r="BL9" s="15"/>
+      <c r="AW9" s="15"/>
       <c r="BM9" s="4"/>
-      <c r="BR9" s="15"/>
-      <c r="BS9" s="15"/>
       <c r="BT9" s="4"/>
-      <c r="BU9" s="15"/>
-      <c r="BV9" s="15"/>
-      <c r="BW9" s="15"/>
       <c r="BX9" s="4"/>
       <c r="BZ9" s="4"/>
-      <c r="CA9" s="18"/>
-      <c r="CN9" s="15"/>
-      <c r="CO9" s="15"/>
+      <c r="CA9" s="15"/>
       <c r="CQ9" s="4"/>
-      <c r="CU9" s="15"/>
-      <c r="CV9" s="15"/>
-      <c r="CW9" s="15"/>
       <c r="CX9" s="4"/>
-      <c r="CZ9" s="15"/>
       <c r="DB9" s="4"/>
       <c r="DD9" s="4"/>
-      <c r="DE9" s="18"/>
-      <c r="DL9" s="15"/>
-      <c r="DQ9" s="15"/>
-      <c r="DS9" s="15"/>
+      <c r="DE9" s="15"/>
       <c r="DU9" s="4"/>
-      <c r="DW9" s="15"/>
-      <c r="DX9" s="15"/>
-      <c r="DY9" s="15"/>
       <c r="EB9" s="4"/>
       <c r="EF9" s="4"/>
       <c r="EH9" s="4"/>
-      <c r="EI9" s="18"/>
-      <c r="EJ9" s="15"/>
-      <c r="EK9" s="15"/>
-      <c r="EL9" s="15"/>
-      <c r="EM9" s="15"/>
-      <c r="EN9" s="15"/>
-      <c r="EO9" s="15"/>
-      <c r="EP9" s="15"/>
-      <c r="EQ9" s="15"/>
-      <c r="ER9" s="15"/>
-      <c r="ES9" s="15"/>
-      <c r="ET9" s="15"/>
-      <c r="EU9" s="15"/>
-      <c r="EV9" s="15"/>
-      <c r="EW9" s="15"/>
-      <c r="EX9" s="15"/>
-      <c r="EY9" s="15"/>
-      <c r="EZ9" s="15"/>
-      <c r="FA9" s="15"/>
-      <c r="FB9" s="15"/>
-      <c r="FC9" s="15"/>
-      <c r="FD9" s="15"/>
-      <c r="FE9" s="15"/>
-      <c r="FF9" s="15"/>
-      <c r="FG9" s="15"/>
-      <c r="FH9" s="15"/>
-      <c r="FI9" s="15"/>
-      <c r="FJ9" s="15"/>
-      <c r="FK9" s="15"/>
-      <c r="FL9" s="15"/>
-      <c r="FM9" s="15"/>
-      <c r="FN9" s="15"/>
-      <c r="FO9" s="15"/>
-      <c r="FP9" s="15"/>
-      <c r="FQ9" s="15"/>
-      <c r="FR9" s="15"/>
-      <c r="FS9" s="15"/>
-      <c r="FT9" s="15"/>
-      <c r="FU9" s="15"/>
-      <c r="FV9" s="15"/>
-      <c r="FW9" s="15"/>
-      <c r="FX9" s="15"/>
-      <c r="FY9" s="15"/>
-      <c r="FZ9" s="15"/>
-      <c r="GA9" s="15"/>
-      <c r="GB9" s="15"/>
-      <c r="GC9" s="15"/>
-      <c r="GD9" s="15"/>
-      <c r="GE9" s="15"/>
-      <c r="GF9" s="15"/>
-      <c r="GG9" s="15"/>
-      <c r="GH9" s="15"/>
-      <c r="GI9" s="15"/>
-      <c r="GJ9" s="15"/>
-      <c r="GK9" s="15"/>
-      <c r="GL9" s="15"/>
-      <c r="GM9" s="15"/>
-      <c r="GN9" s="15"/>
-      <c r="GO9" s="15"/>
-      <c r="GP9" s="15"/>
-      <c r="GQ9" s="15"/>
-      <c r="GR9" s="15"/>
-      <c r="GS9" s="15"/>
-      <c r="GT9" s="15"/>
-      <c r="GU9" s="15"/>
-      <c r="GV9" s="15"/>
-      <c r="GW9" s="15"/>
-      <c r="GX9" s="15"/>
-      <c r="GY9" s="15"/>
-      <c r="GZ9" s="15"/>
-      <c r="HA9" s="15"/>
-      <c r="HB9" s="15"/>
-      <c r="HC9" s="15"/>
-      <c r="HD9" s="15"/>
-      <c r="HE9" s="15"/>
-      <c r="HF9" s="15"/>
-      <c r="HG9" s="15"/>
-      <c r="HH9" s="15"/>
-      <c r="HI9" s="15"/>
-      <c r="HJ9" s="15"/>
-      <c r="HK9" s="15"/>
-      <c r="HL9" s="15"/>
-      <c r="HM9" s="15"/>
-      <c r="HN9" s="15"/>
-      <c r="HO9" s="15"/>
-      <c r="HP9" s="15"/>
-      <c r="HQ9" s="15"/>
-      <c r="HR9" s="15"/>
-      <c r="HS9" s="15"/>
-      <c r="HT9" s="15"/>
-      <c r="HU9" s="15"/>
-      <c r="HV9" s="15"/>
-      <c r="HW9" s="15"/>
-      <c r="HX9" s="15"/>
-      <c r="HY9" s="15"/>
-      <c r="HZ9" s="15"/>
-      <c r="IA9" s="15"/>
-      <c r="IB9" s="15"/>
-      <c r="IC9" s="15"/>
-      <c r="ID9" s="15"/>
-      <c r="IE9" s="15"/>
-      <c r="IF9" s="15"/>
-      <c r="IG9" s="15"/>
-      <c r="IH9" s="15"/>
-      <c r="II9" s="15"/>
-      <c r="IJ9" s="15"/>
-      <c r="IK9" s="15"/>
-      <c r="IL9" s="15"/>
-      <c r="IM9" s="15"/>
-      <c r="IN9" s="15"/>
-      <c r="IO9" s="15"/>
-      <c r="IP9" s="15"/>
-      <c r="IQ9" s="15"/>
-      <c r="IR9" s="15"/>
-      <c r="IS9" s="15"/>
-      <c r="IT9" s="15"/>
-      <c r="IU9" s="15"/>
-      <c r="IV9" s="15"/>
-      <c r="IW9" s="15"/>
-      <c r="IX9" s="15"/>
-      <c r="IY9" s="15"/>
-      <c r="IZ9" s="15"/>
-      <c r="JA9" s="15"/>
-      <c r="JB9" s="15"/>
-      <c r="JC9" s="15"/>
-      <c r="JD9" s="15"/>
-      <c r="JE9" s="15"/>
-      <c r="JF9" s="15"/>
-      <c r="JG9" s="15"/>
-      <c r="JH9" s="15"/>
-      <c r="JI9" s="15"/>
-      <c r="JJ9" s="15"/>
-      <c r="JK9" s="15"/>
-      <c r="JL9" s="15"/>
-      <c r="JM9" s="15"/>
-      <c r="JN9" s="15"/>
-      <c r="JO9" s="15"/>
-      <c r="JP9" s="15"/>
-      <c r="JQ9" s="15"/>
-      <c r="JR9" s="15"/>
-      <c r="JS9" s="15"/>
-      <c r="JT9" s="15"/>
-      <c r="JU9" s="15"/>
-      <c r="JV9" s="15"/>
-      <c r="JW9" s="15"/>
+      <c r="EI9" s="15"/>
+      <c r="EJ9" s="5"/>
+      <c r="EK9" s="19"/>
+      <c r="EL9" s="19"/>
+      <c r="EM9" s="4"/>
+      <c r="EN9" s="19"/>
+      <c r="EO9" s="19"/>
+      <c r="EP9" s="19"/>
+      <c r="EQ9" s="19"/>
+      <c r="ER9" s="19"/>
+      <c r="ES9" s="19"/>
+      <c r="ET9" s="19"/>
+      <c r="EU9" s="19"/>
+      <c r="EV9" s="19"/>
+      <c r="EW9" s="19"/>
+      <c r="EX9" s="19"/>
+      <c r="EY9" s="19"/>
+      <c r="EZ9" s="19"/>
+      <c r="FA9" s="19"/>
+      <c r="FB9" s="19"/>
+      <c r="FC9" s="4"/>
     </row>
-    <row r="10" spans="1:283" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:278" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8"/>
       <c r="C10" s="9"/>
       <c r="S10" s="9"/>
@@ -4690,174 +3614,579 @@
       <c r="EF10" s="8"/>
       <c r="EH10" s="8"/>
       <c r="EI10" s="10"/>
-      <c r="EJ10" s="15"/>
-      <c r="EK10" s="15"/>
-      <c r="EL10" s="15"/>
-      <c r="EM10" s="15"/>
-      <c r="EN10" s="15"/>
-      <c r="EO10" s="15"/>
-      <c r="EP10" s="15"/>
-      <c r="EQ10" s="15"/>
-      <c r="ER10" s="15"/>
-      <c r="ES10" s="15"/>
-      <c r="ET10" s="15"/>
-      <c r="EU10" s="15"/>
-      <c r="EV10" s="15"/>
-      <c r="EW10" s="15"/>
-      <c r="EX10" s="15"/>
-      <c r="EY10" s="15"/>
-      <c r="EZ10" s="15"/>
-      <c r="FA10" s="15"/>
-      <c r="FB10" s="15"/>
-      <c r="FC10" s="15"/>
-      <c r="FD10" s="15"/>
-      <c r="FE10" s="15"/>
-      <c r="FF10" s="15"/>
-      <c r="FG10" s="15"/>
-      <c r="FH10" s="15"/>
-      <c r="FI10" s="15"/>
-      <c r="FJ10" s="15"/>
-      <c r="FK10" s="15"/>
-      <c r="FL10" s="15"/>
-      <c r="FM10" s="15"/>
-      <c r="FN10" s="15"/>
-      <c r="FO10" s="15"/>
-      <c r="FP10" s="15"/>
-      <c r="FQ10" s="15"/>
-      <c r="FR10" s="15"/>
-      <c r="FS10" s="15"/>
-      <c r="FT10" s="15"/>
-      <c r="FU10" s="15"/>
-      <c r="FV10" s="15"/>
-      <c r="FW10" s="15"/>
-      <c r="FX10" s="15"/>
-      <c r="FY10" s="15"/>
-      <c r="FZ10" s="15"/>
-      <c r="GA10" s="15"/>
-      <c r="GB10" s="15"/>
-      <c r="GC10" s="15"/>
-      <c r="GD10" s="15"/>
-      <c r="GE10" s="15"/>
-      <c r="GF10" s="15"/>
-      <c r="GG10" s="15"/>
-      <c r="GH10" s="15"/>
-      <c r="GI10" s="15"/>
-      <c r="GJ10" s="15"/>
-      <c r="GK10" s="15"/>
-      <c r="GL10" s="15"/>
-      <c r="GM10" s="15"/>
-      <c r="GN10" s="15"/>
-      <c r="GO10" s="15"/>
-      <c r="GP10" s="15"/>
-      <c r="GQ10" s="15"/>
-      <c r="GR10" s="15"/>
-      <c r="GS10" s="15"/>
-      <c r="GT10" s="15"/>
-      <c r="GU10" s="15"/>
-      <c r="GV10" s="15"/>
-      <c r="GW10" s="15"/>
-      <c r="GX10" s="15"/>
-      <c r="GY10" s="15"/>
-      <c r="GZ10" s="15"/>
-      <c r="HA10" s="15"/>
-      <c r="HB10" s="15"/>
-      <c r="HC10" s="15"/>
-      <c r="HD10" s="15"/>
-      <c r="HE10" s="15"/>
-      <c r="HF10" s="15"/>
-      <c r="HG10" s="15"/>
-      <c r="HH10" s="15"/>
-      <c r="HI10" s="15"/>
-      <c r="HJ10" s="15"/>
-      <c r="HK10" s="15"/>
-      <c r="HL10" s="15"/>
-      <c r="HM10" s="15"/>
-      <c r="HN10" s="15"/>
-      <c r="HO10" s="15"/>
-      <c r="HP10" s="15"/>
-      <c r="HQ10" s="15"/>
-      <c r="HR10" s="15"/>
-      <c r="HS10" s="15"/>
-      <c r="HT10" s="15"/>
-      <c r="HU10" s="15"/>
-      <c r="HV10" s="15"/>
-      <c r="HW10" s="15"/>
-      <c r="HX10" s="15"/>
-      <c r="HY10" s="15"/>
-      <c r="HZ10" s="15"/>
-      <c r="IA10" s="15"/>
-      <c r="IB10" s="15"/>
-      <c r="IC10" s="15"/>
-      <c r="ID10" s="15"/>
-      <c r="IE10" s="15"/>
-      <c r="IF10" s="15"/>
-      <c r="IG10" s="15"/>
-      <c r="IH10" s="15"/>
-      <c r="II10" s="15"/>
-      <c r="IJ10" s="15"/>
-      <c r="IK10" s="15"/>
-      <c r="IL10" s="15"/>
-      <c r="IM10" s="15"/>
-      <c r="IN10" s="15"/>
-      <c r="IO10" s="15"/>
-      <c r="IP10" s="15"/>
-      <c r="IQ10" s="15"/>
-      <c r="IR10" s="15"/>
-      <c r="IS10" s="15"/>
-      <c r="IT10" s="15"/>
-      <c r="IU10" s="15"/>
-      <c r="IV10" s="15"/>
-      <c r="IW10" s="15"/>
-      <c r="IX10" s="15"/>
-      <c r="IY10" s="15"/>
-      <c r="IZ10" s="15"/>
-      <c r="JA10" s="15"/>
-      <c r="JB10" s="15"/>
-      <c r="JC10" s="15"/>
-      <c r="JD10" s="15"/>
-      <c r="JE10" s="15"/>
-      <c r="JF10" s="15"/>
-      <c r="JG10" s="15"/>
-      <c r="JH10" s="15"/>
-      <c r="JI10" s="15"/>
-      <c r="JJ10" s="15"/>
-      <c r="JK10" s="15"/>
-      <c r="JL10" s="15"/>
-      <c r="JM10" s="15"/>
-      <c r="JN10" s="15"/>
-      <c r="JO10" s="15"/>
-      <c r="JP10" s="15"/>
-      <c r="JQ10" s="15"/>
-      <c r="JR10" s="15"/>
-      <c r="JS10" s="15"/>
-      <c r="JT10" s="15"/>
-      <c r="JU10" s="15"/>
-      <c r="JV10" s="15"/>
-      <c r="JW10" s="15"/>
+      <c r="EJ10" s="9"/>
+      <c r="EM10" s="8"/>
+      <c r="FC10" s="8"/>
+      <c r="FD10"/>
+      <c r="FE10"/>
+      <c r="FF10"/>
+      <c r="FG10"/>
+      <c r="FH10"/>
+      <c r="FI10"/>
+      <c r="FJ10"/>
+      <c r="FK10"/>
+      <c r="FL10"/>
+      <c r="FM10"/>
+      <c r="FN10"/>
+      <c r="FO10"/>
+      <c r="FP10"/>
+      <c r="FQ10"/>
+      <c r="FR10"/>
+      <c r="FS10"/>
+      <c r="FT10"/>
+      <c r="FU10"/>
+      <c r="FV10"/>
+      <c r="FW10"/>
+      <c r="FX10"/>
+      <c r="FY10"/>
+      <c r="FZ10"/>
+      <c r="GA10"/>
+      <c r="GB10"/>
+      <c r="GC10"/>
+      <c r="GD10"/>
+      <c r="GE10"/>
+      <c r="GF10"/>
+      <c r="GG10"/>
+      <c r="GH10"/>
+      <c r="GI10"/>
+      <c r="GJ10"/>
+      <c r="GK10"/>
+      <c r="GL10"/>
+      <c r="GM10"/>
+      <c r="GN10"/>
+      <c r="GO10"/>
+      <c r="GP10"/>
+      <c r="GQ10"/>
+      <c r="GR10"/>
+      <c r="GS10"/>
+      <c r="GT10"/>
+      <c r="GU10"/>
+      <c r="GV10"/>
+      <c r="GW10"/>
+      <c r="GX10"/>
+      <c r="GY10"/>
+      <c r="GZ10"/>
+      <c r="HA10"/>
+      <c r="HB10"/>
+      <c r="HC10"/>
+      <c r="HD10"/>
+      <c r="HE10"/>
+      <c r="HF10"/>
+      <c r="HG10"/>
+      <c r="HH10"/>
+      <c r="HI10"/>
+      <c r="HJ10"/>
+      <c r="HK10"/>
+      <c r="HL10"/>
+      <c r="HM10"/>
+      <c r="HN10"/>
+      <c r="HO10"/>
+      <c r="HP10"/>
+      <c r="HQ10"/>
+      <c r="HR10"/>
+      <c r="HS10"/>
+      <c r="HT10"/>
+      <c r="HU10"/>
+      <c r="HV10"/>
+      <c r="HW10"/>
+      <c r="HX10"/>
+      <c r="HY10"/>
+      <c r="HZ10"/>
+      <c r="IA10"/>
+      <c r="IB10"/>
+      <c r="IC10"/>
+      <c r="ID10"/>
+      <c r="IE10"/>
+      <c r="IF10"/>
+      <c r="IG10"/>
+      <c r="IH10"/>
+      <c r="II10"/>
+      <c r="IJ10"/>
+      <c r="IK10"/>
+      <c r="IL10"/>
+      <c r="IM10"/>
+      <c r="IN10"/>
+      <c r="IO10"/>
+      <c r="IP10"/>
+      <c r="IQ10"/>
+      <c r="IR10"/>
+      <c r="IS10"/>
+      <c r="IT10"/>
+      <c r="IU10"/>
+      <c r="IV10"/>
+      <c r="IW10"/>
+      <c r="IX10"/>
+      <c r="IY10"/>
+      <c r="IZ10"/>
+      <c r="JA10"/>
+      <c r="JB10"/>
+      <c r="JC10"/>
+      <c r="JD10"/>
+      <c r="JE10"/>
+      <c r="JF10"/>
+      <c r="JG10"/>
+      <c r="JH10"/>
+      <c r="JI10"/>
+      <c r="JJ10"/>
+      <c r="JK10"/>
+      <c r="JL10"/>
+      <c r="JM10"/>
+      <c r="JN10"/>
+      <c r="JO10"/>
+      <c r="JP10"/>
+      <c r="JQ10"/>
+      <c r="JR10"/>
     </row>
-    <row r="11" spans="1:283" x14ac:dyDescent="0.35">
-      <c r="DS11" s="15"/>
+    <row r="11" spans="1:278" x14ac:dyDescent="0.35">
+      <c r="FC11" s="19"/>
     </row>
-    <row r="13" spans="1:283" x14ac:dyDescent="0.35">
-      <c r="BW13" s="15"/>
-      <c r="BX13" s="15"/>
-    </row>
-    <row r="14" spans="1:283" x14ac:dyDescent="0.35">
-      <c r="DS14" s="15"/>
-    </row>
-    <row r="15" spans="1:283" x14ac:dyDescent="0.35">
-      <c r="DS15" s="15"/>
+    <row r="12" spans="1:278" x14ac:dyDescent="0.35">
+      <c r="FC12" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F4770D-06D5-479C-B775-EA20CAF83085}">
+  <dimension ref="A1:EI1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:139" x14ac:dyDescent="0.35">
+      <c r="A1" s="4">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1">
+        <v>183934904</v>
+      </c>
+      <c r="H1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I1">
+        <v>92879</v>
+      </c>
+      <c r="J1">
+        <v>5</v>
+      </c>
+      <c r="K1">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1">
+        <v>9232003</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1">
+        <v>1638493959</v>
+      </c>
+      <c r="P1" s="1">
+        <v>1727838499</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2893930406</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="S1" s="5">
+        <v>92879</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="U1">
+        <v>2</v>
+      </c>
+      <c r="V1" t="s">
+        <v>219</v>
+      </c>
+      <c r="W1" t="s">
+        <v>218</v>
+      </c>
+      <c r="X1">
+        <v>450000</v>
+      </c>
+      <c r="Y1" s="4">
+        <v>540000</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE1">
+        <v>345000</v>
+      </c>
+      <c r="AF1">
+        <v>15</v>
+      </c>
+      <c r="AG1">
+        <v>7</v>
+      </c>
+      <c r="AH1">
+        <v>240</v>
+      </c>
+      <c r="AI1" s="4">
+        <v>240</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>208</v>
+      </c>
+      <c r="AK1">
+        <v>92879</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AM1">
+        <v>7</v>
+      </c>
+      <c r="AN1">
+        <v>7</v>
+      </c>
+      <c r="AO1">
+        <v>25678</v>
+      </c>
+      <c r="AP1" s="13">
+        <v>4091997</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AT1" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>246</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="AW1" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>211</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BB1" s="1">
+        <v>189309305</v>
+      </c>
+      <c r="BC1" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="BD1">
+        <v>92879</v>
+      </c>
+      <c r="BE1">
+        <v>6</v>
+      </c>
+      <c r="BF1">
+        <v>2</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>44</v>
+      </c>
+      <c r="BH1">
+        <v>12121992</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>31</v>
+      </c>
+      <c r="BJ1">
+        <v>1738299349</v>
+      </c>
+      <c r="BK1">
+        <v>5273493596</v>
+      </c>
+      <c r="BL1">
+        <v>7632874985</v>
+      </c>
+      <c r="BM1" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>215</v>
+      </c>
+      <c r="BP1">
+        <v>92879</v>
+      </c>
+      <c r="BQ1">
+        <v>8</v>
+      </c>
+      <c r="BR1">
+        <v>9</v>
+      </c>
+      <c r="BS1">
+        <v>7182006</v>
+      </c>
+      <c r="BT1" s="4">
+        <v>20918</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>220</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>240</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>227</v>
+      </c>
+      <c r="BX1" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="BY1" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="BZ1" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="CA1" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>86</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>9</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>87</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CF1">
+        <v>210987654</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>162</v>
+      </c>
+      <c r="CH1">
+        <v>92879</v>
+      </c>
+      <c r="CI1">
+        <v>6</v>
+      </c>
+      <c r="CJ1">
+        <v>7</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="CL1" s="1">
+        <v>4091997</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="CN1" s="1">
+        <v>8725378554</v>
+      </c>
+      <c r="CO1" s="1">
+        <v>6778901234</v>
+      </c>
+      <c r="CP1" s="1">
+        <v>8912345678</v>
+      </c>
+      <c r="CQ1" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>172</v>
+      </c>
+      <c r="CS1">
+        <v>3291998</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>194</v>
+      </c>
+      <c r="CU1">
+        <v>92879</v>
+      </c>
+      <c r="CV1">
+        <v>15</v>
+      </c>
+      <c r="CW1">
+        <v>2</v>
+      </c>
+      <c r="CX1">
+        <v>34000</v>
+      </c>
+      <c r="CY1" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>240</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>227</v>
+      </c>
+      <c r="DB1" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>247</v>
+      </c>
+      <c r="DD1" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="DE1" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>89</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>93</v>
+      </c>
+      <c r="DJ1">
+        <v>901234567</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>164</v>
+      </c>
+      <c r="DL1">
+        <v>92879</v>
+      </c>
+      <c r="DM1">
+        <v>2</v>
+      </c>
+      <c r="DN1">
+        <v>4</v>
+      </c>
+      <c r="DO1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="DP1" s="1">
+        <v>12122006</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="DR1" s="1">
+        <v>7183829496</v>
+      </c>
+      <c r="DS1" s="1">
+        <v>8902736475</v>
+      </c>
+      <c r="DT1" s="1">
+        <v>4536789102</v>
+      </c>
+      <c r="DU1" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="DV1" t="s">
+        <v>170</v>
+      </c>
+      <c r="DW1" s="1">
+        <v>7282003</v>
+      </c>
+      <c r="DX1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="DY1" s="1">
+        <v>92879</v>
+      </c>
+      <c r="DZ1" s="1">
+        <v>9</v>
+      </c>
+      <c r="EA1" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB1" s="17">
+        <v>29000</v>
+      </c>
+      <c r="EC1" t="s">
+        <v>220</v>
+      </c>
+      <c r="ED1" t="s">
+        <v>224</v>
+      </c>
+      <c r="EE1" t="s">
+        <v>227</v>
+      </c>
+      <c r="EF1" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="EG1" t="s">
+        <v>247</v>
+      </c>
+      <c r="EH1" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="EI1" s="15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
   <hyperlinks>
-    <hyperlink ref="R2" r:id="rId1" xr:uid="{802F9EAE-4E42-42A5-91C1-73E04449F74E}"/>
+    <hyperlink ref="R1" r:id="rId1" xr:uid="{802F9EAE-4E42-42A5-91C1-73E04449F74E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D8D4ED-8A60-4C2E-917D-9E135735BD8A}">
   <dimension ref="A1:R3"/>
   <sheetViews>
@@ -5061,7 +4390,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69843AF8-0002-40F4-B634-22AD064CC4DF}">
   <dimension ref="A1:J3"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated encompass.js, encompass.spec.js and NewLoan.xlsx
</commit_message>
<xml_diff>
--- a/test_Data/Loan.xlsx
+++ b/test_Data/Loan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NagaSaiSriharshaKara\Desktop\PRMG\test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7111AAC8-63BC-48EC-980C-046256A967B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5FC850-91BA-4E7E-912D-F5925FD43A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="2" xr2:uid="{162BA2F1-E430-497A-A5CB-FF5EFBDA5730}"/>
   </bookViews>
@@ -16,9 +16,8 @@
     <sheet name="Borrower Information" sheetId="1" r:id="rId1"/>
     <sheet name="Property Title" sheetId="3" r:id="rId2"/>
     <sheet name="Loans Info" sheetId="6" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
-    <sheet name="Employment Income" sheetId="5" r:id="rId5"/>
-    <sheet name="Loan Information" sheetId="4" r:id="rId6"/>
+    <sheet name="Employment Income" sheetId="5" r:id="rId4"/>
+    <sheet name="Loan Information" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="282">
   <si>
     <t>First Name</t>
   </si>
@@ -675,9 +674,6 @@
   </si>
   <si>
     <t>Tsarukyan</t>
-  </si>
-  <si>
-    <t>432 street</t>
   </si>
   <si>
     <t>arman@gmail.com</t>
@@ -1033,7 +1029,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1047,9 +1043,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -1071,11 +1064,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1394,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C103B7CF-E5A8-4494-B4BF-C49089A5F3DF}">
   <dimension ref="A1:AH9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1782,7 +1778,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1901,66 +1897,65 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{442BC2CD-504F-478A-8238-60A656DB3140}">
-  <dimension ref="A1:JR12"/>
+  <dimension ref="A1:JR10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="BB6" sqref="BB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.6328125" customWidth="1"/>
+    <col min="11" max="11" width="7.453125" customWidth="1"/>
+    <col min="12" max="12" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.54296875" customWidth="1"/>
+    <col min="22" max="22" width="10.36328125" customWidth="1"/>
+    <col min="23" max="23" width="8.36328125" customWidth="1"/>
+    <col min="24" max="24" width="9.1796875" customWidth="1"/>
+    <col min="25" max="25" width="9.08984375" customWidth="1"/>
+    <col min="26" max="26" width="8.36328125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="8" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.6328125" customWidth="1"/>
+    <col min="30" max="30" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.26953125" customWidth="1"/>
     <col min="32" max="32" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.26953125" customWidth="1"/>
+    <col min="36" max="36" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="7.81640625" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="18.08984375" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="6.1796875" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="15" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.453125" customWidth="1"/>
     <col min="54" max="54" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="7.36328125" bestFit="1" customWidth="1"/>
@@ -2069,482 +2064,482 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:278" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="W1" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="W1" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="Z1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AA1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AB1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AC1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AD1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="11" t="s">
+      <c r="AE1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AF1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="11" t="s">
+      <c r="AG1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AH1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="12" t="s">
+      <c r="AI1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AK1" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AL1" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AM1" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="AN1" s="6" t="s">
+      <c r="AN1" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="AO1" s="6" t="s">
+      <c r="AO1" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="AP1" s="8" t="s">
+      <c r="AP1" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="AQ1" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="AR1" s="6" t="s">
+      <c r="AQ1" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="AS1" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="AT1" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="AU1" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="AV1" s="8" t="s">
+      <c r="AR1" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="AS1" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT1" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU1" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="AV1" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AW1" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="AX1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AY1" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="AZ1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="BA1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="BB1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="BC1" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD1" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="BE1" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="BF1" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="BG1" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="BH1" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="BI1" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="BJ1" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="BK1" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="BL1" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="BM1" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="BN1" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="BO1" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="BP1" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="BQ1" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="BR1" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="BS1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="BT1" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="BU1" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="BV1" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="BW1" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="BX1" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="BY1" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="BZ1" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="AW1" s="10" t="s">
+      <c r="CA1" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="AX1" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="AY1" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="AZ1" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="BA1" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="BB1" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="BC1" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="BD1" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="BE1" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="BF1" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="BG1" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="BH1" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="BI1" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="BJ1" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="BK1" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="BL1" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="BM1" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="BN1" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="BO1" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="BP1" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="BQ1" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="BR1" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="BS1" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="BT1" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="BU1" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="BV1" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="BW1" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="BX1" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="BY1" s="9" t="s">
+      <c r="CB1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="CC1" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="CD1" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="CE1" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="CF1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="CG1" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="CH1" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="CI1" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="CJ1" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="CK1" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="CL1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="CM1" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="CN1" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="CO1" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="CP1" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="CQ1" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="CR1" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="CS1" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="CT1" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="CU1" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="CV1" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="CW1" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="CX1" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="CY1" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="CZ1" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="DA1" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="DB1" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="DC1" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="BZ1" s="8" t="s">
+      <c r="DD1" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="CA1" s="10" t="s">
+      <c r="DE1" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="DF1" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="DG1" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="DH1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="DI1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="DJ1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="DK1" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="DL1" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="DM1" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="DN1" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="DO1" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="DP1" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="DQ1" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="DR1" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="DS1" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="DT1" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="DU1" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="DV1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="DW1" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="DX1" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="DY1" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="DZ1" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="EA1" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="EB1" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="EC1" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="ED1" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="EE1" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="EF1" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="EG1" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="EH1" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="EI1" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="EJ1" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="CB1" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="CC1" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="CD1" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="CE1" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="CF1" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="CG1" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="CH1" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="CI1" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="CJ1" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="CK1" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="CL1" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="CM1" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="CN1" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="CO1" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="CP1" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="CQ1" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="CR1" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="CS1" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="CT1" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="CU1" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="CV1" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="CW1" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="CX1" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="CY1" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="CZ1" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="DA1" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="DB1" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="DC1" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="DD1" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="DE1" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="DF1" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="DG1" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="DH1" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="DI1" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="DJ1" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="DK1" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="DL1" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="DM1" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="DN1" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="DO1" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="DP1" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="DQ1" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="DR1" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="DS1" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="DT1" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="DU1" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="DV1" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="DW1" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="DX1" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="DY1" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="DZ1" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="EA1" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="EB1" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="EC1" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="ED1" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="EE1" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="EF1" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="EG1" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="EH1" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="EI1" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="EJ1" s="6" t="s">
+      <c r="EK1" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="EK1" s="6" t="s">
+      <c r="EL1" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="EL1" s="6" t="s">
+      <c r="EM1" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="EM1" s="8" t="s">
+      <c r="EN1" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="EN1" s="6" t="s">
+      <c r="EO1" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="EO1" s="6" t="s">
+      <c r="EP1" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="EP1" s="6" t="s">
+      <c r="EQ1" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="EQ1" s="6" t="s">
+      <c r="ER1" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="ER1" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="ES1" s="6" t="s">
+      <c r="ES1" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="ET1" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="ET1" s="6" t="s">
+      <c r="EU1" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="EU1" s="6" t="s">
+      <c r="EV1" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="EV1" s="6" t="s">
+      <c r="EW1" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="EW1" s="6" t="s">
+      <c r="EX1" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="EX1" s="6" t="s">
+      <c r="EY1" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="EY1" s="6" t="s">
+      <c r="EZ1" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="EZ1" s="6" t="s">
+      <c r="FA1" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="FA1" s="6" t="s">
+      <c r="FB1" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="FB1" s="6" t="s">
+      <c r="FC1" s="11" t="s">
         <v>279</v>
-      </c>
-      <c r="FC1" s="8" t="s">
-        <v>280</v>
       </c>
       <c r="FD1"/>
       <c r="FE1"/>
@@ -2718,7 +2713,7 @@
       <c r="Q2" s="1">
         <v>2893930406</v>
       </c>
-      <c r="R2" s="20" t="s">
+      <c r="R2" t="s">
         <v>206</v>
       </c>
       <c r="S2" s="5">
@@ -2731,10 +2726,10 @@
         <v>2</v>
       </c>
       <c r="V2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="X2">
         <v>450000</v>
@@ -2790,29 +2785,29 @@
       <c r="AO2">
         <v>25678</v>
       </c>
-      <c r="AP2" s="13">
+      <c r="AP2" s="12">
         <v>4091997</v>
       </c>
       <c r="AQ2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AR2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AS2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AT2" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AU2" t="s">
+        <v>245</v>
+      </c>
+      <c r="AV2" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="AV2" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="AW2" s="15" t="s">
-        <v>246</v>
+      <c r="AW2" s="14" t="s">
+        <v>245</v>
       </c>
       <c r="AX2" t="s">
         <v>210</v>
@@ -2829,8 +2824,8 @@
       <c r="BB2" s="1">
         <v>189309305</v>
       </c>
-      <c r="BC2" s="22" t="s">
-        <v>282</v>
+      <c r="BC2" s="18" t="s">
+        <v>281</v>
       </c>
       <c r="BD2">
         <v>92879</v>
@@ -2859,14 +2854,14 @@
       <c r="BL2">
         <v>7632874985</v>
       </c>
-      <c r="BM2" s="14" t="s">
+      <c r="BM2" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="BN2" t="s">
         <v>213</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="BO2" t="s">
         <v>214</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>215</v>
       </c>
       <c r="BP2">
         <v>92879</v>
@@ -2884,25 +2879,25 @@
         <v>20918</v>
       </c>
       <c r="BU2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="BV2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="BW2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="BX2" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="BY2" s="16" t="s">
-        <v>247</v>
+        <v>229</v>
+      </c>
+      <c r="BY2" s="15" t="s">
+        <v>246</v>
       </c>
       <c r="BZ2" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="CA2" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
+      </c>
+      <c r="CA2" s="14" t="s">
+        <v>246</v>
       </c>
       <c r="CB2" t="s">
         <v>86</v>
@@ -2973,26 +2968,26 @@
       <c r="CX2">
         <v>34000</v>
       </c>
-      <c r="CY2" s="16" t="s">
-        <v>220</v>
+      <c r="CY2" s="15" t="s">
+        <v>219</v>
       </c>
       <c r="CZ2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="DA2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="DB2" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="DC2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="DD2" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="DE2" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
+      </c>
+      <c r="DE2" s="14" t="s">
+        <v>246</v>
       </c>
       <c r="DF2" t="s">
         <v>88</v>
@@ -3060,50 +3055,50 @@
       <c r="EA2" s="1">
         <v>0</v>
       </c>
-      <c r="EB2" s="17">
+      <c r="EB2" s="16">
         <v>29000</v>
       </c>
       <c r="EC2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="ED2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="EE2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="EF2" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>246</v>
+      </c>
+      <c r="EH2" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="EI2" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>219</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>239</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>226</v>
+      </c>
+      <c r="EM2" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="EG2" t="s">
-        <v>247</v>
-      </c>
-      <c r="EH2" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="EI2" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>220</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>240</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>227</v>
-      </c>
-      <c r="EM2" s="4" t="s">
-        <v>231</v>
-      </c>
       <c r="EN2" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="EO2" t="s">
         <v>9</v>
       </c>
       <c r="EP2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="EQ2" t="s">
         <v>90</v>
@@ -3141,8 +3136,8 @@
       <c r="FB2" s="1">
         <v>2893930406</v>
       </c>
-      <c r="FC2" s="21" t="s">
-        <v>281</v>
+      <c r="FC2" s="13" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:278" x14ac:dyDescent="0.35">
@@ -3188,7 +3183,7 @@
       <c r="N3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3" s="17">
         <v>1111111111</v>
       </c>
       <c r="P3" s="1">
@@ -3210,10 +3205,10 @@
         <v>1</v>
       </c>
       <c r="V3" t="s">
+        <v>217</v>
+      </c>
+      <c r="W3" t="s">
         <v>218</v>
-      </c>
-      <c r="W3" t="s">
-        <v>219</v>
       </c>
       <c r="X3">
         <v>420000</v>
@@ -3273,25 +3268,25 @@
         <v>8092014</v>
       </c>
       <c r="AQ3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AR3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AS3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AT3" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AU3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AV3" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="AW3" s="14" t="s">
         <v>246</v>
-      </c>
-      <c r="AW3" s="15" t="s">
-        <v>247</v>
       </c>
       <c r="AX3" t="s">
         <v>84</v>
@@ -3329,13 +3324,13 @@
       <c r="BI3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="BJ3" s="18">
+      <c r="BJ3" s="17">
         <v>9999999999</v>
       </c>
-      <c r="BK3" s="18">
+      <c r="BK3" s="17">
         <v>8888888888</v>
       </c>
-      <c r="BL3" s="18">
+      <c r="BL3" s="17">
         <v>7777777777</v>
       </c>
       <c r="BM3" s="4" t="s">
@@ -3363,36 +3358,36 @@
         <v>26500</v>
       </c>
       <c r="BU3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="BV3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="BW3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="BX3" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="BY3" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="BZ3" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="CA3" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="CA3" s="14" t="s">
+        <v>245</v>
       </c>
       <c r="CR3" s="5"/>
       <c r="CY3" s="5"/>
       <c r="DB3" s="4"/>
       <c r="DD3" s="4"/>
-      <c r="DE3" s="15"/>
+      <c r="DE3" s="14"/>
       <c r="DU3" s="4"/>
       <c r="EB3" s="4"/>
       <c r="EF3" s="4"/>
       <c r="EH3" s="4"/>
-      <c r="EI3" s="15"/>
+      <c r="EI3" s="14"/>
       <c r="EM3" s="4"/>
       <c r="FC3" s="4"/>
     </row>
@@ -3406,22 +3401,22 @@
       <c r="AP4" s="4"/>
       <c r="AT4" s="4"/>
       <c r="AV4" s="4"/>
-      <c r="AW4" s="15"/>
+      <c r="AW4" s="14"/>
       <c r="BM4" s="4"/>
       <c r="BT4" s="4"/>
       <c r="BX4" s="4"/>
       <c r="BZ4" s="4"/>
-      <c r="CA4" s="15"/>
+      <c r="CA4" s="14"/>
       <c r="CQ4" s="4"/>
       <c r="CX4" s="4"/>
       <c r="DB4" s="4"/>
       <c r="DD4" s="4"/>
-      <c r="DE4" s="15"/>
+      <c r="DE4" s="14"/>
       <c r="DU4" s="4"/>
       <c r="EB4" s="4"/>
       <c r="EF4" s="4"/>
       <c r="EH4" s="4"/>
-      <c r="EI4" s="15"/>
+      <c r="EI4" s="14"/>
       <c r="EM4" s="4"/>
       <c r="FC4" s="4"/>
     </row>
@@ -3435,22 +3430,22 @@
       <c r="AP5" s="4"/>
       <c r="AT5" s="4"/>
       <c r="AV5" s="4"/>
-      <c r="AW5" s="15"/>
+      <c r="AW5" s="14"/>
       <c r="BM5" s="4"/>
       <c r="BT5" s="4"/>
       <c r="BX5" s="4"/>
       <c r="BZ5" s="4"/>
-      <c r="CA5" s="15"/>
+      <c r="CA5" s="14"/>
       <c r="CQ5" s="4"/>
       <c r="CX5" s="4"/>
       <c r="DB5" s="4"/>
       <c r="DD5" s="4"/>
-      <c r="DE5" s="15"/>
+      <c r="DE5" s="14"/>
       <c r="DU5" s="4"/>
       <c r="EB5" s="4"/>
       <c r="EF5" s="4"/>
       <c r="EH5" s="4"/>
-      <c r="EI5" s="15"/>
+      <c r="EI5" s="14"/>
       <c r="EM5" s="4"/>
       <c r="FC5" s="4"/>
     </row>
@@ -3464,22 +3459,22 @@
       <c r="AP6" s="4"/>
       <c r="AT6" s="4"/>
       <c r="AV6" s="4"/>
-      <c r="AW6" s="15"/>
+      <c r="AW6" s="14"/>
       <c r="BM6" s="4"/>
       <c r="BT6" s="4"/>
       <c r="BX6" s="4"/>
       <c r="BZ6" s="4"/>
-      <c r="CA6" s="15"/>
+      <c r="CA6" s="14"/>
       <c r="CQ6" s="4"/>
       <c r="CX6" s="4"/>
       <c r="DB6" s="4"/>
       <c r="DD6" s="4"/>
-      <c r="DE6" s="15"/>
+      <c r="DE6" s="14"/>
       <c r="DU6" s="4"/>
       <c r="EB6" s="4"/>
       <c r="EF6" s="4"/>
       <c r="EH6" s="4"/>
-      <c r="EI6" s="15"/>
+      <c r="EI6" s="14"/>
       <c r="EM6" s="4"/>
       <c r="FC6" s="4"/>
     </row>
@@ -3493,22 +3488,22 @@
       <c r="AP7" s="4"/>
       <c r="AT7" s="4"/>
       <c r="AV7" s="4"/>
-      <c r="AW7" s="15"/>
+      <c r="AW7" s="14"/>
       <c r="BM7" s="4"/>
       <c r="BT7" s="4"/>
       <c r="BX7" s="4"/>
       <c r="BZ7" s="4"/>
-      <c r="CA7" s="15"/>
+      <c r="CA7" s="14"/>
       <c r="CQ7" s="4"/>
       <c r="CX7" s="4"/>
       <c r="DB7" s="4"/>
       <c r="DD7" s="4"/>
-      <c r="DE7" s="15"/>
+      <c r="DE7" s="14"/>
       <c r="DU7" s="4"/>
       <c r="EB7" s="4"/>
       <c r="EF7" s="4"/>
       <c r="EH7" s="4"/>
-      <c r="EI7" s="15"/>
+      <c r="EI7" s="14"/>
       <c r="EM7" s="4"/>
       <c r="FC7" s="4"/>
     </row>
@@ -3522,22 +3517,22 @@
       <c r="AP8" s="4"/>
       <c r="AT8" s="4"/>
       <c r="AV8" s="4"/>
-      <c r="AW8" s="15"/>
+      <c r="AW8" s="14"/>
       <c r="BM8" s="4"/>
       <c r="BT8" s="4"/>
       <c r="BX8" s="4"/>
       <c r="BZ8" s="4"/>
-      <c r="CA8" s="15"/>
+      <c r="CA8" s="14"/>
       <c r="CQ8" s="4"/>
       <c r="CX8" s="4"/>
       <c r="DB8" s="4"/>
       <c r="DD8" s="4"/>
-      <c r="DE8" s="15"/>
+      <c r="DE8" s="14"/>
       <c r="DU8" s="4"/>
       <c r="EB8" s="4"/>
       <c r="EF8" s="4"/>
       <c r="EH8" s="4"/>
-      <c r="EI8" s="15"/>
+      <c r="EI8" s="14"/>
       <c r="EM8" s="4"/>
       <c r="FC8" s="4"/>
     </row>
@@ -3551,72 +3546,55 @@
       <c r="AP9" s="4"/>
       <c r="AT9" s="4"/>
       <c r="AV9" s="4"/>
-      <c r="AW9" s="15"/>
+      <c r="AW9" s="14"/>
       <c r="BM9" s="4"/>
       <c r="BT9" s="4"/>
       <c r="BX9" s="4"/>
       <c r="BZ9" s="4"/>
-      <c r="CA9" s="15"/>
+      <c r="CA9" s="14"/>
       <c r="CQ9" s="4"/>
       <c r="CX9" s="4"/>
       <c r="DB9" s="4"/>
       <c r="DD9" s="4"/>
-      <c r="DE9" s="15"/>
+      <c r="DE9" s="14"/>
       <c r="DU9" s="4"/>
       <c r="EB9" s="4"/>
       <c r="EF9" s="4"/>
       <c r="EH9" s="4"/>
-      <c r="EI9" s="15"/>
+      <c r="EI9" s="14"/>
       <c r="EJ9" s="5"/>
-      <c r="EK9" s="19"/>
-      <c r="EL9" s="19"/>
       <c r="EM9" s="4"/>
-      <c r="EN9" s="19"/>
-      <c r="EO9" s="19"/>
-      <c r="EP9" s="19"/>
-      <c r="EQ9" s="19"/>
-      <c r="ER9" s="19"/>
-      <c r="ES9" s="19"/>
-      <c r="ET9" s="19"/>
-      <c r="EU9" s="19"/>
-      <c r="EV9" s="19"/>
-      <c r="EW9" s="19"/>
-      <c r="EX9" s="19"/>
-      <c r="EY9" s="19"/>
-      <c r="EZ9" s="19"/>
-      <c r="FA9" s="19"/>
-      <c r="FB9" s="19"/>
       <c r="FC9" s="4"/>
     </row>
     <row r="10" spans="1:278" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="9"/>
-      <c r="AI10" s="8"/>
-      <c r="AP10" s="8"/>
-      <c r="AT10" s="8"/>
-      <c r="AV10" s="8"/>
-      <c r="AW10" s="10"/>
-      <c r="BM10" s="8"/>
-      <c r="BT10" s="8"/>
-      <c r="BX10" s="8"/>
-      <c r="BZ10" s="8"/>
-      <c r="CA10" s="10"/>
-      <c r="CQ10" s="8"/>
-      <c r="CX10" s="8"/>
-      <c r="DB10" s="8"/>
-      <c r="DD10" s="8"/>
-      <c r="DE10" s="10"/>
-      <c r="DU10" s="8"/>
-      <c r="EB10" s="8"/>
-      <c r="EF10" s="8"/>
-      <c r="EH10" s="8"/>
-      <c r="EI10" s="10"/>
-      <c r="EJ10" s="9"/>
-      <c r="EM10" s="8"/>
-      <c r="FC10" s="8"/>
+      <c r="A10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="8"/>
+      <c r="AI10" s="7"/>
+      <c r="AP10" s="7"/>
+      <c r="AT10" s="7"/>
+      <c r="AV10" s="7"/>
+      <c r="AW10" s="9"/>
+      <c r="BM10" s="7"/>
+      <c r="BT10" s="7"/>
+      <c r="BX10" s="7"/>
+      <c r="BZ10" s="7"/>
+      <c r="CA10" s="9"/>
+      <c r="CQ10" s="7"/>
+      <c r="CX10" s="7"/>
+      <c r="DB10" s="7"/>
+      <c r="DD10" s="7"/>
+      <c r="DE10" s="9"/>
+      <c r="DU10" s="7"/>
+      <c r="EB10" s="7"/>
+      <c r="EF10" s="7"/>
+      <c r="EH10" s="7"/>
+      <c r="EI10" s="9"/>
+      <c r="EJ10" s="8"/>
+      <c r="EM10" s="7"/>
+      <c r="FC10" s="7"/>
       <c r="FD10"/>
       <c r="FE10"/>
       <c r="FF10"/>
@@ -3737,12 +3715,6 @@
       <c r="JQ10"/>
       <c r="JR10"/>
     </row>
-    <row r="11" spans="1:278" x14ac:dyDescent="0.35">
-      <c r="FC11" s="19"/>
-    </row>
-    <row r="12" spans="1:278" x14ac:dyDescent="0.35">
-      <c r="FC12" s="19"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3750,448 +3722,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F4770D-06D5-479C-B775-EA20CAF83085}">
-  <dimension ref="A1:EI1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:139" x14ac:dyDescent="0.35">
-      <c r="A1" s="4">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>2</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1">
-        <v>183934904</v>
-      </c>
-      <c r="H1" t="s">
-        <v>205</v>
-      </c>
-      <c r="I1">
-        <v>92879</v>
-      </c>
-      <c r="J1">
-        <v>5</v>
-      </c>
-      <c r="K1">
-        <v>3</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1">
-        <v>9232003</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O1">
-        <v>1638493959</v>
-      </c>
-      <c r="P1" s="1">
-        <v>1727838499</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>2893930406</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="S1" s="5">
-        <v>92879</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="U1">
-        <v>2</v>
-      </c>
-      <c r="V1" t="s">
-        <v>219</v>
-      </c>
-      <c r="W1" t="s">
-        <v>218</v>
-      </c>
-      <c r="X1">
-        <v>450000</v>
-      </c>
-      <c r="Y1" s="4">
-        <v>540000</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE1">
-        <v>345000</v>
-      </c>
-      <c r="AF1">
-        <v>15</v>
-      </c>
-      <c r="AG1">
-        <v>7</v>
-      </c>
-      <c r="AH1">
-        <v>240</v>
-      </c>
-      <c r="AI1" s="4">
-        <v>240</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>208</v>
-      </c>
-      <c r="AK1">
-        <v>92879</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>209</v>
-      </c>
-      <c r="AM1">
-        <v>7</v>
-      </c>
-      <c r="AN1">
-        <v>7</v>
-      </c>
-      <c r="AO1">
-        <v>25678</v>
-      </c>
-      <c r="AP1" s="13">
-        <v>4091997</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>220</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>240</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>227</v>
-      </c>
-      <c r="AT1" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>246</v>
-      </c>
-      <c r="AV1" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="AW1" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>210</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>211</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="BB1" s="1">
-        <v>189309305</v>
-      </c>
-      <c r="BC1" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="BD1">
-        <v>92879</v>
-      </c>
-      <c r="BE1">
-        <v>6</v>
-      </c>
-      <c r="BF1">
-        <v>2</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>44</v>
-      </c>
-      <c r="BH1">
-        <v>12121992</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BJ1">
-        <v>1738299349</v>
-      </c>
-      <c r="BK1">
-        <v>5273493596</v>
-      </c>
-      <c r="BL1">
-        <v>7632874985</v>
-      </c>
-      <c r="BM1" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>214</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>215</v>
-      </c>
-      <c r="BP1">
-        <v>92879</v>
-      </c>
-      <c r="BQ1">
-        <v>8</v>
-      </c>
-      <c r="BR1">
-        <v>9</v>
-      </c>
-      <c r="BS1">
-        <v>7182006</v>
-      </c>
-      <c r="BT1" s="4">
-        <v>20918</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>220</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>240</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>227</v>
-      </c>
-      <c r="BX1" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="BY1" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="BZ1" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="CA1" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>86</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>9</v>
-      </c>
-      <c r="CD1" t="s">
-        <v>87</v>
-      </c>
-      <c r="CE1" t="s">
-        <v>91</v>
-      </c>
-      <c r="CF1">
-        <v>210987654</v>
-      </c>
-      <c r="CG1" t="s">
-        <v>162</v>
-      </c>
-      <c r="CH1">
-        <v>92879</v>
-      </c>
-      <c r="CI1">
-        <v>6</v>
-      </c>
-      <c r="CJ1">
-        <v>7</v>
-      </c>
-      <c r="CK1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="CL1" s="1">
-        <v>4091997</v>
-      </c>
-      <c r="CM1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="CN1" s="1">
-        <v>8725378554</v>
-      </c>
-      <c r="CO1" s="1">
-        <v>6778901234</v>
-      </c>
-      <c r="CP1" s="1">
-        <v>8912345678</v>
-      </c>
-      <c r="CQ1" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>172</v>
-      </c>
-      <c r="CS1">
-        <v>3291998</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>194</v>
-      </c>
-      <c r="CU1">
-        <v>92879</v>
-      </c>
-      <c r="CV1">
-        <v>15</v>
-      </c>
-      <c r="CW1">
-        <v>2</v>
-      </c>
-      <c r="CX1">
-        <v>34000</v>
-      </c>
-      <c r="CY1" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>240</v>
-      </c>
-      <c r="DA1" t="s">
-        <v>227</v>
-      </c>
-      <c r="DB1" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="DC1" t="s">
-        <v>247</v>
-      </c>
-      <c r="DD1" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="DE1" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="DF1" t="s">
-        <v>88</v>
-      </c>
-      <c r="DG1" t="s">
-        <v>9</v>
-      </c>
-      <c r="DH1" t="s">
-        <v>89</v>
-      </c>
-      <c r="DI1" t="s">
-        <v>93</v>
-      </c>
-      <c r="DJ1">
-        <v>901234567</v>
-      </c>
-      <c r="DK1" t="s">
-        <v>164</v>
-      </c>
-      <c r="DL1">
-        <v>92879</v>
-      </c>
-      <c r="DM1">
-        <v>2</v>
-      </c>
-      <c r="DN1">
-        <v>4</v>
-      </c>
-      <c r="DO1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="DP1" s="1">
-        <v>12122006</v>
-      </c>
-      <c r="DQ1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="DR1" s="1">
-        <v>7183829496</v>
-      </c>
-      <c r="DS1" s="1">
-        <v>8902736475</v>
-      </c>
-      <c r="DT1" s="1">
-        <v>4536789102</v>
-      </c>
-      <c r="DU1" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="DV1" t="s">
-        <v>170</v>
-      </c>
-      <c r="DW1" s="1">
-        <v>7282003</v>
-      </c>
-      <c r="DX1" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="DY1" s="1">
-        <v>92879</v>
-      </c>
-      <c r="DZ1" s="1">
-        <v>9</v>
-      </c>
-      <c r="EA1" s="1">
-        <v>0</v>
-      </c>
-      <c r="EB1" s="17">
-        <v>29000</v>
-      </c>
-      <c r="EC1" t="s">
-        <v>220</v>
-      </c>
-      <c r="ED1" t="s">
-        <v>224</v>
-      </c>
-      <c r="EE1" t="s">
-        <v>227</v>
-      </c>
-      <c r="EF1" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="EG1" t="s">
-        <v>247</v>
-      </c>
-      <c r="EH1" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="EI1" s="15" t="s">
-        <v>247</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="R1" r:id="rId1" xr:uid="{802F9EAE-4E42-42A5-91C1-73E04449F74E}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D8D4ED-8A60-4C2E-917D-9E135735BD8A}">
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4390,12 +3925,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69843AF8-0002-40F4-B634-22AD064CC4DF}">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added macro based excel NewLoan.xlsm and modified encompass spec file accordingly
</commit_message>
<xml_diff>
--- a/test_Data/Loan.xlsx
+++ b/test_Data/Loan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NagaSaiSriharshaKara\Desktop\PRMG\test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5FC850-91BA-4E7E-912D-F5925FD43A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5543A2A7-B09C-4FCF-991C-43C32D6AF6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="2" xr2:uid="{162BA2F1-E430-497A-A5CB-FF5EFBDA5730}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{162BA2F1-E430-497A-A5CB-FF5EFBDA5730}"/>
   </bookViews>
   <sheets>
     <sheet name="Borrower Information" sheetId="1" r:id="rId1"/>
@@ -1390,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C103B7CF-E5A8-4494-B4BF-C49089A5F3DF}">
   <dimension ref="A1:AH9"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1899,7 +1899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{442BC2CD-504F-478A-8238-60A656DB3140}">
   <dimension ref="A1:JR10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
+    <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="BB6" sqref="BB6"/>
     </sheetView>
   </sheetViews>

</xml_diff>